<commit_message>
seventh update: updating electricity mix in 2021
</commit_message>
<xml_diff>
--- a/database/calliope_generators.xlsx
+++ b/database/calliope_generators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_power_system\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0163A7-5E05-46E7-A770-90C31D4D483A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C328CC-C960-46FF-893D-7D3489E4A6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
   </bookViews>
@@ -19,6 +19,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>bus</t>
   </si>
@@ -263,15 +264,49 @@
   <si>
     <t>factor</t>
   </si>
+  <si>
+    <t>RUPTL 2021-30</t>
+  </si>
+  <si>
+    <t>ruptl 2021</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>south,central</t>
+  </si>
+  <si>
+    <t>east,north</t>
+  </si>
+  <si>
+    <t>LCOE Capacity full report</t>
+  </si>
+  <si>
+    <t>assumption factor</t>
+  </si>
+  <si>
+    <t>total cap</t>
+  </si>
+  <si>
+    <t>demand ratio</t>
+  </si>
+  <si>
+    <t>electrification ratio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,8 +322,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Abadi Extra Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +425,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,10 +602,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -733,28 +795,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -773,8 +814,44 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -796,6 +873,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>178592</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323467</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>15715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{885FE5DC-A8D9-46C0-9155-88C8684496A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4822030"/>
+          <a:ext cx="9530808" cy="4119563"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -2885,6 +3011,60 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="pypsa"/>
+      <sheetName val="calliope_1"/>
+      <sheetName val="calliope_2"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="-jr28gpurfjy0ufw0"/>
+      <sheetName val="-jr28gpurfjy0ufw0 (2)"/>
+      <sheetName val="-jr28gpurfjy0ufw0 (3)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="L2">
+            <v>352.95152055845813</v>
+          </cell>
+          <cell r="M2">
+            <v>213.5804325130739</v>
+          </cell>
+          <cell r="N2">
+            <v>325.86064954249946</v>
+          </cell>
+          <cell r="O2">
+            <v>429.07122508811278</v>
+          </cell>
+          <cell r="P2">
+            <v>79.958862020278815</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="D11">
+            <v>370.10844748858648</v>
+          </cell>
+          <cell r="E11">
+            <v>565.6632420091338</v>
+          </cell>
+          <cell r="F11">
+            <v>531.15514126215476</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3187,75 +3367,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83E7F3-B837-43E6-BF88-00ED77709958}">
-  <dimension ref="A1:AN47"/>
+  <dimension ref="A1:AY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AQ25" sqref="AQ25"/>
+      <selection pane="bottomRight" activeCell="BA14" sqref="BA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.109375" style="120" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="5"/>
+    <col min="4" max="4" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="8.88671875" style="120" customWidth="1"/>
     <col min="14" max="23" width="8.88671875" customWidth="1"/>
-    <col min="32" max="40" width="0" hidden="1" customWidth="1"/>
+    <col min="31" max="32" width="8.88671875" customWidth="1"/>
+    <col min="33" max="50" width="8.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="C1" s="128">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="C1" s="143">
         <v>2021</v>
       </c>
-      <c r="D1" s="128"/>
-      <c r="E1" s="129" t="s">
+      <c r="D1" s="143"/>
+      <c r="E1" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="130" t="s">
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="142" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="142"/>
+      <c r="P1" s="142"/>
+      <c r="Q1" s="142"/>
+      <c r="R1" s="142"/>
+      <c r="S1" s="142"/>
+      <c r="T1" s="142"/>
+      <c r="U1" s="142"/>
+      <c r="V1" s="142"/>
+      <c r="W1" s="145" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="145"/>
+      <c r="Y1" s="145"/>
+      <c r="Z1" s="145"/>
+      <c r="AA1" s="145"/>
+      <c r="AB1" s="145"/>
+      <c r="AC1" s="145"/>
+      <c r="AD1" s="145"/>
+      <c r="AE1" s="145"/>
+      <c r="AF1" s="128"/>
+      <c r="AG1" s="142" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH1" s="142"/>
+      <c r="AI1" s="142"/>
+      <c r="AJ1" s="142"/>
+      <c r="AK1" s="142"/>
+      <c r="AL1" s="142"/>
+      <c r="AM1" s="142"/>
+      <c r="AN1" s="142"/>
+      <c r="AO1" s="142"/>
+      <c r="AP1" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="130"/>
-      <c r="W1" s="131" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="131"/>
-      <c r="Y1" s="131"/>
-      <c r="Z1" s="131"/>
-      <c r="AA1" s="131"/>
-      <c r="AB1" s="131"/>
-      <c r="AC1" s="131"/>
-      <c r="AD1" s="131"/>
-      <c r="AE1" s="131"/>
-      <c r="AF1" s="130" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG1" s="130"/>
-      <c r="AH1" s="130"/>
-      <c r="AI1" s="130"/>
-      <c r="AJ1" s="130"/>
-      <c r="AK1" s="130"/>
-      <c r="AL1" s="130"/>
-      <c r="AM1" s="130"/>
-      <c r="AN1" s="130"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ1" s="142"/>
+      <c r="AR1" s="142"/>
+      <c r="AS1" s="142"/>
+      <c r="AT1" s="142"/>
+      <c r="AU1" s="142"/>
+      <c r="AV1" s="142"/>
+      <c r="AW1" s="142"/>
+      <c r="AX1" s="142"/>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3349,35 +3542,65 @@
       <c r="AE2" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="101" t="s">
+      <c r="AF2" s="140" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG2" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="AG2" s="102" t="s">
+      <c r="AH2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="103" t="s">
+      <c r="AI2" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="104" t="s">
+      <c r="AJ2" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="AJ2" s="105" t="s">
+      <c r="AK2" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="106" t="s">
+      <c r="AL2" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="AL2" s="107" t="s">
+      <c r="AM2" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="AM2" s="108" t="s">
+      <c r="AN2" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="AN2" s="109" t="s">
+      <c r="AO2" s="109" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AP2" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ2" s="102" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS2" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT2" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU2" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="AV2" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW2" s="108" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX2" s="109" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" s="126">
         <v>0.86423333300000005</v>
       </c>
@@ -3418,22 +3641,22 @@
         <v>0</v>
       </c>
       <c r="N3" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O3" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P3" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q3" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R3" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S3" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T3" s="116">
         <v>1</v>
@@ -3450,7 +3673,7 @@
       </c>
       <c r="X3" s="111">
         <f t="shared" si="0"/>
-        <v>142.5</v>
+        <v>117.5</v>
       </c>
       <c r="Y3" s="112">
         <f t="shared" si="0"/>
@@ -3466,7 +3689,7 @@
       </c>
       <c r="AB3" s="115">
         <f t="shared" si="0"/>
-        <v>9.0860899999999987</v>
+        <v>1.71899</v>
       </c>
       <c r="AC3" s="116">
         <f t="shared" si="0"/>
@@ -3480,35 +3703,63 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF3" s="110">
+      <c r="AF3" s="141"/>
+      <c r="AG3" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG3" s="111">
+      <c r="AH3" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH3" s="112">
+      <c r="AI3" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI3" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="114">
+      <c r="AJ3" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK3" s="115">
+      <c r="AL3" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL3" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM3" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN3" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM3" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ3" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR3" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS3" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT3" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU3" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV3" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" s="126">
         <v>4.5260000000000002E-2</v>
       </c>
@@ -3551,22 +3802,22 @@
         <v>0</v>
       </c>
       <c r="N4" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O4" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P4" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q4" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R4" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S4" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T4" s="116">
         <v>1</v>
@@ -3579,7 +3830,7 @@
       </c>
       <c r="W4" s="110">
         <f t="shared" ref="W4:W22" si="1">E4*N4</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="X4" s="111">
         <f t="shared" ref="X4:X22" si="2">F4*O4</f>
@@ -3599,7 +3850,7 @@
       </c>
       <c r="AB4" s="115">
         <f t="shared" ref="AB4:AB22" si="6">J4*S4</f>
-        <v>49.818650000000005</v>
+        <v>9.4251500000000021</v>
       </c>
       <c r="AC4" s="116">
         <f t="shared" ref="AC4:AC22" si="7">K4*T4</f>
@@ -3613,35 +3864,63 @@
         <f t="shared" ref="AE4:AE22" si="9">M4*V4</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="110">
+      <c r="AF4" s="141"/>
+      <c r="AG4" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG4" s="111">
+      <c r="AH4" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH4" s="112">
+      <c r="AI4" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI4" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="114">
+      <c r="AJ4" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK4" s="115">
+      <c r="AL4" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL4" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM4" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ4" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR4" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS4" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT4" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU4" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV4" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" s="126">
         <v>1.1174249999999999</v>
       </c>
@@ -3685,22 +3964,22 @@
         <v>0</v>
       </c>
       <c r="N5" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O5" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P5" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q5" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R5" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S5" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T5" s="116">
         <v>1</v>
@@ -3717,7 +3996,7 @@
       </c>
       <c r="X5" s="111">
         <f t="shared" si="2"/>
-        <v>62.699999999999996</v>
+        <v>51.699999999999996</v>
       </c>
       <c r="Y5" s="112">
         <f t="shared" si="3"/>
@@ -3729,11 +4008,11 @@
       </c>
       <c r="AA5" s="114">
         <f t="shared" si="5"/>
-        <v>3.76675</v>
+        <v>2.5772500000000003</v>
       </c>
       <c r="AB5" s="115">
         <f t="shared" si="6"/>
-        <v>2.8271699999999997</v>
+        <v>0.53486999999999996</v>
       </c>
       <c r="AC5" s="116">
         <f t="shared" si="7"/>
@@ -3747,35 +4026,65 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF5" s="110">
+      <c r="AF5" s="141">
+        <v>90</v>
+      </c>
+      <c r="AG5" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG5" s="111">
+      <c r="AH5" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH5" s="112">
+      <c r="AI5" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI5" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="114">
+      <c r="AJ5" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK5" s="115">
+      <c r="AL5" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL5" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM5" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP5" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ5" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR5" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS5" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT5" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU5" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV5" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" s="126">
         <v>0.17745</v>
       </c>
@@ -3802,8 +4111,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="114">
-        <f>'[1]Sheet 1'!$F$54</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="J6" s="115">
         <f>'[1]Sheet 1'!$F$49+'[1]Sheet 1'!$F$63+'[1]Sheet 1'!$F$69+'[1]Sheet 1'!$F$70+'[1]Sheet 1'!$F$71+'[1]Sheet 1'!$F$77+'[1]Sheet 1'!$F$78+'[1]Sheet 1'!$F$82+'[1]Sheet 1'!$F$83+'[1]Sheet 1'!$F$84+'[1]Sheet 1'!$F$85+'[1]Sheet 1'!$F$86+'[1]Sheet 1'!$F$87+'[1]Sheet 1'!$F$88+'[1]Sheet 1'!$F$92+'[1]Sheet 1'!$F$93+'[1]Sheet 1'!$F$94+'[1]Sheet 1'!$F$95+'[1]Sheet 1'!$F$96+'[1]Sheet 1'!$F$97+'[1]Sheet 1'!$F$99+'[1]Sheet 1'!$F$100+'[1]Sheet 1'!$F$101+'[1]Sheet 1'!$F$118+'[1]Sheet 1'!$F$119+'[1]Sheet 1'!$F$120+'[1]Sheet 1'!$F$123+'[1]Sheet 1'!$F$124+'[1]Sheet 1'!$F$125+'[1]Sheet 1'!$F$126+'[1]Sheet 1'!$F$127+'[1]Sheet 1'!$F$129+'[1]Sheet 1'!$F$130+'[1]Sheet 1'!$F$131+'[1]Sheet 1'!$F$132+'[1]Sheet 1'!$F$133+'[1]Sheet 1'!$F$134+'[1]Sheet 1'!$F$135+'[1]Sheet 1'!$F$136+'[1]Sheet 1'!$F$137</f>
@@ -3820,22 +4128,22 @@
         <v>0</v>
       </c>
       <c r="N6" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O6" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P6" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q6" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R6" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S6" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T6" s="116">
         <v>1</v>
@@ -3852,7 +4160,7 @@
       </c>
       <c r="X6" s="111">
         <f t="shared" si="2"/>
-        <v>15.389999999999999</v>
+        <v>12.69</v>
       </c>
       <c r="Y6" s="112">
         <f t="shared" si="3"/>
@@ -3863,12 +4171,11 @@
         <v>0</v>
       </c>
       <c r="AA6" s="114">
-        <f t="shared" si="5"/>
-        <v>85.5</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="115">
         <f t="shared" si="6"/>
-        <v>26.031719999999996</v>
+        <v>4.9249200000000002</v>
       </c>
       <c r="AC6" s="116">
         <f t="shared" si="7"/>
@@ -3882,35 +4189,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF6" s="110">
+      <c r="AF6" s="141"/>
+      <c r="AG6" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG6" s="111">
+      <c r="AH6" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH6" s="112">
+      <c r="AI6" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI6" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="114">
+      <c r="AJ6" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK6" s="115">
+      <c r="AL6" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL6" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM6" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ6" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR6" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS6" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT6" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU6" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV6" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" s="126">
         <v>6.3899999999999998E-2</v>
       </c>
@@ -3953,22 +4288,22 @@
         <v>0</v>
       </c>
       <c r="N7" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O7" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P7" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q7" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R7" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S7" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T7" s="116">
         <v>1</v>
@@ -3981,7 +4316,7 @@
       </c>
       <c r="W7" s="110">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="X7" s="111">
         <f t="shared" si="2"/>
@@ -3989,7 +4324,7 @@
       </c>
       <c r="Y7" s="112">
         <f t="shared" si="3"/>
-        <v>12.58</v>
+        <v>18.700000000000003</v>
       </c>
       <c r="Z7" s="113">
         <f t="shared" si="4"/>
@@ -4001,7 +4336,7 @@
       </c>
       <c r="AB7" s="115">
         <f t="shared" si="6"/>
-        <v>61.603520000000003</v>
+        <v>11.654720000000001</v>
       </c>
       <c r="AC7" s="116">
         <f t="shared" si="7"/>
@@ -4015,35 +4350,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF7" s="110">
+      <c r="AF7" s="141"/>
+      <c r="AG7" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG7" s="111">
+      <c r="AH7" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH7" s="112">
+      <c r="AI7" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI7" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="114">
+      <c r="AJ7" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK7" s="115">
+      <c r="AL7" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL7" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM7" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN7" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM7" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ7" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR7" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS7" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT7" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU7" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV7" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" s="126">
         <v>-1.7742</v>
       </c>
@@ -4087,22 +4450,22 @@
         <v>0</v>
       </c>
       <c r="N8" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O8" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P8" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q8" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R8" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S8" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T8" s="116">
         <v>1</v>
@@ -4115,11 +4478,11 @@
       </c>
       <c r="W8" s="110">
         <f t="shared" si="1"/>
-        <v>1.2249999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="X8" s="111">
         <f t="shared" si="2"/>
-        <v>27.929999999999996</v>
+        <v>23.029999999999998</v>
       </c>
       <c r="Y8" s="112">
         <f t="shared" si="3"/>
@@ -4131,11 +4494,11 @@
       </c>
       <c r="AA8" s="114">
         <f t="shared" si="5"/>
-        <v>0.28500000000000003</v>
+        <v>0.19500000000000003</v>
       </c>
       <c r="AB8" s="115">
         <f t="shared" si="6"/>
-        <v>36.145670000000003</v>
+        <v>6.8383700000000012</v>
       </c>
       <c r="AC8" s="116">
         <f t="shared" si="7"/>
@@ -4149,35 +4512,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF8" s="110">
+      <c r="AF8" s="141"/>
+      <c r="AG8" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG8" s="111">
+      <c r="AH8" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH8" s="112">
+      <c r="AI8" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI8" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ8" s="114">
+      <c r="AJ8" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK8" s="115">
+      <c r="AL8" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL8" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM8" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN8" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM8" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ8" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR8" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS8" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT8" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU8" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV8" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" s="126">
         <v>-2.6152000000000002</v>
       </c>
@@ -4221,22 +4612,22 @@
         <v>0</v>
       </c>
       <c r="N9" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O9" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P9" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q9" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R9" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S9" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T9" s="116">
         <v>1</v>
@@ -4249,7 +4640,7 @@
       </c>
       <c r="W9" s="110">
         <f t="shared" si="1"/>
-        <v>4.55</v>
+        <v>3.9</v>
       </c>
       <c r="X9" s="111">
         <f t="shared" si="2"/>
@@ -4269,7 +4660,7 @@
       </c>
       <c r="AB9" s="115">
         <f t="shared" si="6"/>
-        <v>29.372819999999997</v>
+        <v>5.5570200000000005</v>
       </c>
       <c r="AC9" s="116">
         <f t="shared" si="7"/>
@@ -4283,35 +4674,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF9" s="110">
+      <c r="AF9" s="141"/>
+      <c r="AG9" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG9" s="111">
+      <c r="AH9" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH9" s="112">
+      <c r="AI9" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI9" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ9" s="114">
+      <c r="AJ9" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK9" s="115">
+      <c r="AL9" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL9" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN9" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM9" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN9" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP9" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ9" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR9" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS9" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT9" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU9" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV9" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW9" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" s="126">
         <v>-2.6220500000000002</v>
       </c>
@@ -4354,22 +4773,22 @@
         <v>0</v>
       </c>
       <c r="N10" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O10" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P10" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q10" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R10" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S10" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T10" s="116">
         <v>1</v>
@@ -4382,7 +4801,7 @@
       </c>
       <c r="W10" s="110">
         <f t="shared" si="1"/>
-        <v>1.54</v>
+        <v>1.32</v>
       </c>
       <c r="X10" s="111">
         <f t="shared" si="2"/>
@@ -4402,7 +4821,7 @@
       </c>
       <c r="AB10" s="115">
         <f t="shared" si="6"/>
-        <v>6.3151600000000006</v>
+        <v>1.1947600000000003</v>
       </c>
       <c r="AC10" s="116">
         <f t="shared" si="7"/>
@@ -4416,35 +4835,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF10" s="110">
+      <c r="AF10" s="141"/>
+      <c r="AG10" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG10" s="111">
+      <c r="AH10" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH10" s="112">
+      <c r="AI10" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI10" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="114">
+      <c r="AJ10" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK10" s="115">
+      <c r="AL10" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL10" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM10" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN10" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM10" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP10" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ10" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR10" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS10" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT10" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU10" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV10" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW10" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX10" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" s="126">
         <v>-2.1166</v>
       </c>
@@ -4487,22 +4934,22 @@
         <v>0</v>
       </c>
       <c r="N11" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O11" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P11" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q11" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R11" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S11" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T11" s="116">
         <v>1</v>
@@ -4519,7 +4966,7 @@
       </c>
       <c r="X11" s="111">
         <f t="shared" si="2"/>
-        <v>131.13875999999999</v>
+        <v>108.13196000000001</v>
       </c>
       <c r="Y11" s="112">
         <f t="shared" si="3"/>
@@ -4535,7 +4982,7 @@
       </c>
       <c r="AB11" s="115">
         <f t="shared" si="6"/>
-        <v>21.79522</v>
+        <v>4.1234200000000003</v>
       </c>
       <c r="AC11" s="116">
         <f t="shared" si="7"/>
@@ -4549,35 +4996,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF11" s="110">
+      <c r="AF11" s="141"/>
+      <c r="AG11" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG11" s="111">
+      <c r="AH11" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH11" s="112">
+      <c r="AI11" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI11" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="114">
+      <c r="AJ11" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK11" s="115">
+      <c r="AL11" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL11" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN11" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM11" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP11" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ11" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR11" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS11" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT11" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU11" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV11" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW11" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX11" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" s="126">
         <v>-2.8550333330000002</v>
       </c>
@@ -4620,22 +5095,22 @@
         <v>0</v>
       </c>
       <c r="N12" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O12" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P12" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q12" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R12" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S12" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T12" s="116">
         <v>1</v>
@@ -4652,7 +5127,7 @@
       </c>
       <c r="X12" s="111">
         <f t="shared" si="2"/>
-        <v>68.399999999999991</v>
+        <v>56.4</v>
       </c>
       <c r="Y12" s="112">
         <f t="shared" si="3"/>
@@ -4668,7 +5143,7 @@
       </c>
       <c r="AB12" s="115">
         <f t="shared" si="6"/>
-        <v>9.4346300000000003</v>
+        <v>1.7849300000000003</v>
       </c>
       <c r="AC12" s="116">
         <f t="shared" si="7"/>
@@ -4682,35 +5157,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF12" s="110">
+      <c r="AF12" s="141"/>
+      <c r="AG12" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG12" s="111">
+      <c r="AH12" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH12" s="112">
+      <c r="AI12" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI12" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ12" s="114">
+      <c r="AJ12" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK12" s="115">
+      <c r="AL12" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL12" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN12" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM12" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ12" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR12" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS12" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT12" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU12" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV12" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" s="126">
         <v>-0.74419999999999997</v>
       </c>
@@ -4754,22 +5257,22 @@
         <v>0</v>
       </c>
       <c r="N13" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O13" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P13" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q13" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R13" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S13" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T13" s="116">
         <v>1</v>
@@ -4786,11 +5289,11 @@
       </c>
       <c r="X13" s="111">
         <f t="shared" si="2"/>
-        <v>3.9899999999999998</v>
+        <v>3.29</v>
       </c>
       <c r="Y13" s="112">
         <f t="shared" si="3"/>
-        <v>57.832479999999997</v>
+        <v>85.967200000000005</v>
       </c>
       <c r="Z13" s="113">
         <f t="shared" si="4"/>
@@ -4802,7 +5305,7 @@
       </c>
       <c r="AB13" s="115">
         <f t="shared" si="6"/>
-        <v>4.2772000000000006</v>
+        <v>0.80920000000000014</v>
       </c>
       <c r="AC13" s="116">
         <f t="shared" si="7"/>
@@ -4816,35 +5319,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF13" s="110">
+      <c r="AF13" s="141"/>
+      <c r="AG13" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG13" s="111">
+      <c r="AH13" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH13" s="112">
+      <c r="AI13" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI13" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="114">
+      <c r="AJ13" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK13" s="115">
+      <c r="AL13" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL13" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM13" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN13" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM13" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ13" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR13" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS13" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT13" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU13" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV13" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" s="126">
         <v>-3.4291333329999998</v>
       </c>
@@ -4889,22 +5420,22 @@
         <v>0</v>
       </c>
       <c r="N14" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O14" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P14" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q14" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R14" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S14" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T14" s="116">
         <v>1</v>
@@ -4917,11 +5448,11 @@
       </c>
       <c r="W14" s="110">
         <f t="shared" si="1"/>
-        <v>0.84</v>
+        <v>0.72</v>
       </c>
       <c r="X14" s="111">
         <f t="shared" si="2"/>
-        <v>58.823999999999998</v>
+        <v>48.503999999999998</v>
       </c>
       <c r="Y14" s="112">
         <f t="shared" si="3"/>
@@ -4933,11 +5464,11 @@
       </c>
       <c r="AA14" s="114">
         <f t="shared" si="5"/>
-        <v>28.5</v>
+        <v>19.5</v>
       </c>
       <c r="AB14" s="115">
         <f t="shared" si="6"/>
-        <v>36.152700000000003</v>
+        <v>6.8397000000000014</v>
       </c>
       <c r="AC14" s="116">
         <f t="shared" si="7"/>
@@ -4951,35 +5482,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF14" s="110">
+      <c r="AF14" s="141"/>
+      <c r="AG14" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG14" s="111">
+      <c r="AH14" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH14" s="112">
+      <c r="AI14" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI14" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ14" s="114">
+      <c r="AJ14" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK14" s="115">
+      <c r="AL14" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL14" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM14" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN14" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM14" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ14" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR14" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS14" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT14" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU14" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV14" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW14" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX14" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" s="126">
         <v>-2.26065</v>
       </c>
@@ -5022,22 +5581,22 @@
         <v>0</v>
       </c>
       <c r="N15" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O15" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P15" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q15" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R15" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S15" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T15" s="116">
         <v>1</v>
@@ -5054,7 +5613,7 @@
       </c>
       <c r="X15" s="111">
         <f t="shared" si="2"/>
-        <v>165.29999999999998</v>
+        <v>136.29999999999998</v>
       </c>
       <c r="Y15" s="112">
         <f t="shared" si="3"/>
@@ -5070,7 +5629,7 @@
       </c>
       <c r="AB15" s="115">
         <f t="shared" si="6"/>
-        <v>9.907119999999999</v>
+        <v>1.8743200000000002</v>
       </c>
       <c r="AC15" s="116">
         <f t="shared" si="7"/>
@@ -5084,35 +5643,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF15" s="110">
+      <c r="AF15" s="141"/>
+      <c r="AG15" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG15" s="111">
+      <c r="AH15" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH15" s="112">
+      <c r="AI15" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI15" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ15" s="114">
+      <c r="AJ15" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK15" s="115">
+      <c r="AL15" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL15" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM15" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN15" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM15" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN15" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ15" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR15" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS15" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT15" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU15" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV15" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW15" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX15" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" s="126">
         <v>-3.5974499999999998</v>
       </c>
@@ -5155,22 +5742,22 @@
         <v>0</v>
       </c>
       <c r="N16" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O16" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P16" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q16" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R16" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S16" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T16" s="116">
         <v>1</v>
@@ -5187,7 +5774,7 @@
       </c>
       <c r="X16" s="111">
         <f t="shared" si="2"/>
-        <v>160.16999999999999</v>
+        <v>132.07</v>
       </c>
       <c r="Y16" s="112">
         <f t="shared" si="3"/>
@@ -5203,7 +5790,7 @@
       </c>
       <c r="AB16" s="115">
         <f t="shared" si="6"/>
-        <v>6.9079000000000006</v>
+        <v>1.3069000000000002</v>
       </c>
       <c r="AC16" s="116">
         <f t="shared" si="7"/>
@@ -5217,35 +5804,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF16" s="110">
+      <c r="AF16" s="141"/>
+      <c r="AG16" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG16" s="111">
+      <c r="AH16" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH16" s="112">
+      <c r="AI16" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI16" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ16" s="114">
+      <c r="AJ16" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK16" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK16" s="115">
+      <c r="AL16" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL16" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM16" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN16" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM16" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO16" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP16" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ16" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR16" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS16" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT16" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU16" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV16" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW16" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX16" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A17" s="126">
         <v>-1.761425</v>
       </c>
@@ -5287,22 +5902,22 @@
         <v>0</v>
       </c>
       <c r="N17" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O17" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P17" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q17" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R17" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S17" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T17" s="116">
         <v>1</v>
@@ -5335,7 +5950,7 @@
       </c>
       <c r="AB17" s="115">
         <f t="shared" si="6"/>
-        <v>8.4100999999999999</v>
+        <v>1.5911000000000002</v>
       </c>
       <c r="AC17" s="116">
         <f t="shared" si="7"/>
@@ -5349,35 +5964,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF17" s="110">
+      <c r="AF17" s="141"/>
+      <c r="AG17" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG17" s="111">
+      <c r="AH17" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH17" s="112">
+      <c r="AI17" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI17" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="114">
+      <c r="AJ17" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK17" s="115">
+      <c r="AL17" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL17" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM17" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN17" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM17" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP17" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ17" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR17" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS17" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT17" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU17" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV17" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX17" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A18" s="126">
         <v>-1.190416667</v>
       </c>
@@ -5421,22 +6064,22 @@
         <v>0</v>
       </c>
       <c r="N18" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O18" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P18" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q18" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R18" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S18" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T18" s="116">
         <v>1</v>
@@ -5453,11 +6096,11 @@
       </c>
       <c r="X18" s="111">
         <f t="shared" si="2"/>
-        <v>151.04999999999998</v>
+        <v>124.55</v>
       </c>
       <c r="Y18" s="112">
         <f t="shared" si="3"/>
-        <v>46.453499999999998</v>
+        <v>69.052500000000009</v>
       </c>
       <c r="Z18" s="113">
         <f t="shared" si="4"/>
@@ -5469,7 +6112,7 @@
       </c>
       <c r="AB18" s="115">
         <f t="shared" si="6"/>
-        <v>43.546779999999998</v>
+        <v>8.2385800000000007</v>
       </c>
       <c r="AC18" s="116">
         <f t="shared" si="7"/>
@@ -5483,35 +6126,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF18" s="110">
+      <c r="AF18" s="141"/>
+      <c r="AG18" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG18" s="111">
+      <c r="AH18" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH18" s="112">
+      <c r="AI18" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI18" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ18" s="114">
+      <c r="AJ18" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK18" s="115">
+      <c r="AL18" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL18" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM18" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN18" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM18" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP18" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ18" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR18" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS18" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT18" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU18" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV18" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX18" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A19" s="126">
         <v>-0.48473333299999999</v>
       </c>
@@ -5556,22 +6227,22 @@
         <v>0</v>
       </c>
       <c r="N19" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O19" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P19" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q19" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R19" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S19" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T19" s="116">
         <v>1</v>
@@ -5584,15 +6255,15 @@
       </c>
       <c r="W19" s="110">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="X19" s="111">
         <f t="shared" si="2"/>
-        <v>240.82499999999999</v>
+        <v>198.57499999999999</v>
       </c>
       <c r="Y19" s="112">
         <f t="shared" si="3"/>
-        <v>3.552</v>
+        <v>5.28</v>
       </c>
       <c r="Z19" s="113">
         <f t="shared" si="4"/>
@@ -5604,7 +6275,7 @@
       </c>
       <c r="AB19" s="115">
         <f t="shared" si="6"/>
-        <v>147.55822000000001</v>
+        <v>27.916420000000006</v>
       </c>
       <c r="AC19" s="116">
         <f t="shared" si="7"/>
@@ -5618,35 +6289,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF19" s="110">
+      <c r="AF19" s="141"/>
+      <c r="AG19" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG19" s="111">
+      <c r="AH19" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH19" s="112">
+      <c r="AI19" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI19" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ19" s="114">
+      <c r="AJ19" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK19" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK19" s="115">
+      <c r="AL19" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL19" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM19" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN19" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM19" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP19" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ19" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR19" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS19" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT19" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU19" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV19" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW19" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX19" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A20" s="126">
         <v>0.31574999999999998</v>
       </c>
@@ -5690,22 +6389,22 @@
         <v>0</v>
       </c>
       <c r="N20" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O20" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P20" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q20" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R20" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S20" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T20" s="116">
         <v>1</v>
@@ -5722,11 +6421,11 @@
       </c>
       <c r="X20" s="111">
         <f t="shared" si="2"/>
-        <v>158.24909999999997</v>
+        <v>130.48609999999999</v>
       </c>
       <c r="Y20" s="112">
         <f t="shared" si="3"/>
-        <v>22.592200000000002</v>
+        <v>33.583000000000006</v>
       </c>
       <c r="Z20" s="113">
         <f t="shared" si="4"/>
@@ -5738,7 +6437,7 @@
       </c>
       <c r="AB20" s="115">
         <f t="shared" si="6"/>
-        <v>12.994399999999999</v>
+        <v>2.4584000000000001</v>
       </c>
       <c r="AC20" s="116">
         <f t="shared" si="7"/>
@@ -5752,35 +6451,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF20" s="110">
+      <c r="AF20" s="141"/>
+      <c r="AG20" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG20" s="111">
+      <c r="AH20" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH20" s="112">
+      <c r="AI20" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI20" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ20" s="114">
+      <c r="AJ20" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK20" s="115">
+      <c r="AL20" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL20" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM20" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN20" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM20" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ20" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR20" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS20" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT20" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU20" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV20" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX20" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A21" s="126">
         <v>1.0532999999999999</v>
       </c>
@@ -5824,22 +6551,22 @@
         <v>0</v>
       </c>
       <c r="N21" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O21" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P21" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q21" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R21" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S21" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T21" s="116">
         <v>1</v>
@@ -5852,11 +6579,11 @@
       </c>
       <c r="W21" s="110">
         <f t="shared" si="1"/>
-        <v>0.28349999999999997</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="X21" s="111">
         <f t="shared" si="2"/>
-        <v>22.229999999999997</v>
+        <v>18.329999999999998</v>
       </c>
       <c r="Y21" s="112">
         <f t="shared" si="3"/>
@@ -5872,7 +6599,7 @@
       </c>
       <c r="AB21" s="115">
         <f t="shared" si="6"/>
-        <v>14.230570000000002</v>
+        <v>2.6922700000000006</v>
       </c>
       <c r="AC21" s="116">
         <f t="shared" si="7"/>
@@ -5886,35 +6613,63 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF21" s="110">
+      <c r="AF21" s="141"/>
+      <c r="AG21" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG21" s="111">
+      <c r="AH21" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH21" s="112">
+      <c r="AI21" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI21" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ21" s="114">
+      <c r="AJ21" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK21" s="115">
+      <c r="AL21" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL21" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM21" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN21" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM21" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP21" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ21" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR21" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS21" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT21" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU21" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV21" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW21" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX21" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A22" s="126">
         <v>3.2987666670000002</v>
       </c>
@@ -5960,22 +6715,22 @@
         <v>0</v>
       </c>
       <c r="N22" s="110">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="O22" s="111">
-        <v>0.56999999999999995</v>
+        <v>0.47</v>
       </c>
       <c r="P22" s="112">
-        <v>0.37</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q22" s="113">
-        <v>0.73</v>
+        <v>0.9</v>
       </c>
       <c r="R22" s="114">
-        <v>0.95</v>
+        <v>0.65</v>
       </c>
       <c r="S22" s="115">
-        <v>0.37</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T22" s="116">
         <v>1</v>
@@ -5992,11 +6747,11 @@
       </c>
       <c r="X22" s="111">
         <f t="shared" si="2"/>
-        <v>8.2649999999999988</v>
+        <v>6.8149999999999995</v>
       </c>
       <c r="Y22" s="112">
         <f t="shared" si="3"/>
-        <v>45.777879999999996</v>
+        <v>68.048199999999994</v>
       </c>
       <c r="Z22" s="113">
         <f t="shared" si="4"/>
@@ -6004,11 +6759,11 @@
       </c>
       <c r="AA22" s="114">
         <f t="shared" si="5"/>
-        <v>0.22799999999999998</v>
+        <v>0.156</v>
       </c>
       <c r="AB22" s="115">
         <f t="shared" si="6"/>
-        <v>45.41713</v>
+        <v>8.5924300000000002</v>
       </c>
       <c r="AC22" s="116">
         <f t="shared" si="7"/>
@@ -6022,41 +6777,69 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AF22" s="110">
+      <c r="AF22" s="141"/>
+      <c r="AG22" s="110">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AG22" s="111">
+      <c r="AH22" s="111">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AH22" s="112">
+      <c r="AI22" s="112">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AI22" s="113">
-        <v>1</v>
-      </c>
-      <c r="AJ22" s="114">
+      <c r="AJ22" s="113">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="114">
         <v>0.33</v>
       </c>
-      <c r="AK22" s="115">
+      <c r="AL22" s="115">
         <v>0.25</v>
       </c>
-      <c r="AL22" s="116">
-        <v>1</v>
-      </c>
-      <c r="AM22" s="117">
-        <v>1</v>
-      </c>
-      <c r="AN22" s="118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AM22" s="116">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="117">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="118">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="110">
+        <v>0.35</v>
+      </c>
+      <c r="AQ22" s="111">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AR22" s="112">
+        <v>0.37</v>
+      </c>
+      <c r="AS22" s="113">
+        <v>0.73</v>
+      </c>
+      <c r="AT22" s="114">
+        <v>0.95</v>
+      </c>
+      <c r="AU22" s="115">
+        <v>0.37</v>
+      </c>
+      <c r="AV22" s="116">
+        <v>1</v>
+      </c>
+      <c r="AW22" s="117">
+        <v>1</v>
+      </c>
+      <c r="AX22" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
       <c r="C23" s="124" t="s">
         <v>60</v>
       </c>
       <c r="D23" s="125">
         <f>SUM(E23:M23)</f>
-        <v>4735.4920000000002</v>
+        <v>4645.4920000000002</v>
       </c>
       <c r="E23" s="123">
         <f>SUM(E3:E22)</f>
@@ -6076,7 +6859,7 @@
       </c>
       <c r="I23" s="123">
         <f t="shared" si="10"/>
-        <v>124.505</v>
+        <v>34.505000000000003</v>
       </c>
       <c r="J23" s="123">
         <f t="shared" si="10"/>
@@ -6096,15 +6879,15 @@
       </c>
       <c r="W23" s="127">
         <f>SUM(W3:W22)</f>
-        <v>14.388499999999997</v>
+        <v>12.333</v>
       </c>
       <c r="X23" s="127">
         <f t="shared" ref="X23:AE23" si="11">SUM(X3:X22)</f>
-        <v>1416.9618599999999</v>
+        <v>1168.3720600000001</v>
       </c>
       <c r="Y23" s="127">
         <f t="shared" si="11"/>
-        <v>188.78806000000003</v>
+        <v>280.6309</v>
       </c>
       <c r="Z23" s="127">
         <f t="shared" si="11"/>
@@ -6112,11 +6895,11 @@
       </c>
       <c r="AA23" s="127">
         <f t="shared" si="11"/>
-        <v>118.27974999999999</v>
+        <v>22.428249999999998</v>
       </c>
       <c r="AB23" s="127">
         <f t="shared" si="11"/>
-        <v>581.8327700000001</v>
+        <v>110.07647</v>
       </c>
       <c r="AC23" s="127">
         <f t="shared" si="11"/>
@@ -6130,11 +6913,15 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="D24" s="141">
-        <f>SUM(W23:AE23)</f>
-        <v>2321.4709399999997</v>
+      <c r="AF23" s="127">
+        <f t="shared" ref="AF23" si="12">SUM(AF3:AF22)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="D24" s="134">
+        <f>SUM(W23:AE23)+AF5</f>
+        <v>1685.0606800000003</v>
       </c>
       <c r="E24" s="123"/>
       <c r="F24" s="123"/>
@@ -6145,8 +6932,75 @@
       <c r="K24" s="123"/>
       <c r="L24" s="123"/>
       <c r="M24" s="123"/>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="V24" s="127">
+        <f>SUM(W24:AF24)</f>
+        <v>100</v>
+      </c>
+      <c r="W24" s="136">
+        <f>W23/$D$24*100</f>
+        <v>0.73190242620817658</v>
+      </c>
+      <c r="X24" s="136">
+        <f t="shared" ref="X24:AF24" si="13">X23/$D$24*100</f>
+        <v>69.337091172289405</v>
+      </c>
+      <c r="Y24" s="136">
+        <f t="shared" si="13"/>
+        <v>16.654053075406161</v>
+      </c>
+      <c r="Z24" s="136">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="136">
+        <f t="shared" si="13"/>
+        <v>1.3310054804673261</v>
+      </c>
+      <c r="AB24" s="136">
+        <f t="shared" si="13"/>
+        <v>6.5324929426280347</v>
+      </c>
+      <c r="AC24" s="136">
+        <f t="shared" si="13"/>
+        <v>7.2400953537174684E-2</v>
+      </c>
+      <c r="AD24" s="136">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="136">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="136">
+        <f t="shared" si="13"/>
+        <v>5.3410539494637064</v>
+      </c>
+      <c r="AG24" s="120"/>
+      <c r="AH24" s="120"/>
+      <c r="AI24" s="120"/>
+      <c r="AJ24" s="120"/>
+      <c r="AK24" s="120"/>
+      <c r="AL24" s="120"/>
+      <c r="AM24" s="120"/>
+      <c r="AN24" s="120"/>
+      <c r="AO24" s="120"/>
+      <c r="AP24" s="120"/>
+      <c r="AQ24" s="120"/>
+      <c r="AR24" s="120"/>
+      <c r="AS24" s="120"/>
+      <c r="AT24" s="120"/>
+      <c r="AU24" s="120"/>
+      <c r="AV24" s="120"/>
+      <c r="AW24" s="120"/>
+      <c r="AX24" s="120"/>
+      <c r="AY24" s="120"/>
+    </row>
+    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="D25" s="135">
+        <f>SUMPRODUCT(E3:M22,AG3:AO22)</f>
+        <v>1424.3024999999996</v>
+      </c>
       <c r="E25" s="123"/>
       <c r="F25" s="123"/>
       <c r="G25" s="123"/>
@@ -6156,8 +7010,61 @@
       <c r="K25" s="123"/>
       <c r="L25" s="123"/>
       <c r="M25" s="123"/>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="V25" t="s">
+        <v>75</v>
+      </c>
+      <c r="W25" s="137">
+        <v>0.52</v>
+      </c>
+      <c r="X25" s="137">
+        <v>68.58</v>
+      </c>
+      <c r="Y25" s="137">
+        <v>16.3</v>
+      </c>
+      <c r="Z25" s="137">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="137">
+        <v>1.04</v>
+      </c>
+      <c r="AB25" s="137">
+        <v>6.73</v>
+      </c>
+      <c r="AC25" s="137">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="137">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="137">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="137">
+        <v>6.82</v>
+      </c>
+      <c r="AG25" s="138"/>
+      <c r="AH25" s="138"/>
+      <c r="AI25" s="138"/>
+      <c r="AJ25" s="138"/>
+      <c r="AK25" s="138"/>
+      <c r="AL25" s="138"/>
+      <c r="AM25" s="138"/>
+      <c r="AN25" s="138"/>
+      <c r="AO25" s="138"/>
+      <c r="AP25" s="138"/>
+      <c r="AQ25" s="138"/>
+      <c r="AR25" s="138"/>
+      <c r="AS25" s="138"/>
+      <c r="AT25" s="138"/>
+      <c r="AU25" s="138"/>
+      <c r="AV25" s="138"/>
+      <c r="AW25" s="138"/>
+      <c r="AX25" s="138"/>
+      <c r="AY25" s="138"/>
+    </row>
+    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="D26" s="135"/>
       <c r="E26" s="123"/>
       <c r="F26" s="123"/>
       <c r="G26" s="123"/>
@@ -6167,41 +7074,417 @@
       <c r="K26" s="123"/>
       <c r="L26" s="123"/>
       <c r="M26" s="123"/>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="123"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="123"/>
-      <c r="M27" s="123"/>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-      <c r="H28" s="123"/>
-      <c r="I28" s="123"/>
-      <c r="J28" s="123"/>
-      <c r="K28" s="123"/>
-      <c r="L28" s="123"/>
-      <c r="M28" s="123"/>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="123"/>
-      <c r="H29" s="123"/>
-      <c r="I29" s="123"/>
-      <c r="J29" s="123"/>
-      <c r="K29" s="123"/>
-      <c r="L29" s="123"/>
-      <c r="M29" s="123"/>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="T26" t="s">
+        <v>84</v>
+      </c>
+      <c r="U26" t="s">
+        <v>83</v>
+      </c>
+      <c r="V26" t="s">
+        <v>82</v>
+      </c>
+      <c r="W26" s="137"/>
+      <c r="X26" s="137"/>
+      <c r="Y26" s="137"/>
+      <c r="Z26" s="137"/>
+      <c r="AA26" s="137"/>
+      <c r="AB26" s="137"/>
+      <c r="AC26" s="137"/>
+      <c r="AD26" s="137"/>
+      <c r="AE26" s="137"/>
+      <c r="AF26" s="137"/>
+      <c r="AG26" s="138"/>
+      <c r="AH26" s="138"/>
+      <c r="AI26" s="138"/>
+      <c r="AJ26" s="138"/>
+      <c r="AK26" s="138"/>
+      <c r="AL26" s="138"/>
+      <c r="AM26" s="138"/>
+      <c r="AN26" s="138"/>
+      <c r="AO26" s="138"/>
+      <c r="AP26" s="138"/>
+      <c r="AQ26" s="138"/>
+      <c r="AR26" s="138"/>
+      <c r="AS26" s="138"/>
+      <c r="AT26" s="138"/>
+      <c r="AU26" s="138"/>
+      <c r="AV26" s="138"/>
+      <c r="AW26" s="138"/>
+      <c r="AX26" s="138"/>
+      <c r="AY26" s="138"/>
+    </row>
+    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="C27" s="120" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="135"/>
+      <c r="E27" s="123">
+        <f>SUM(E3:E8)</f>
+        <v>18.5</v>
+      </c>
+      <c r="F27" s="123">
+        <f t="shared" ref="F27:M27" si="14">SUM(F3:F8)</f>
+        <v>436</v>
+      </c>
+      <c r="G27" s="123">
+        <f t="shared" si="14"/>
+        <v>34</v>
+      </c>
+      <c r="H27" s="123">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="123">
+        <f t="shared" si="14"/>
+        <v>4.2650000000000006</v>
+      </c>
+      <c r="J27" s="123">
+        <f t="shared" si="14"/>
+        <v>501.38599999999997</v>
+      </c>
+      <c r="K27" s="123">
+        <f t="shared" si="14"/>
+        <v>0.18</v>
+      </c>
+      <c r="L27" s="123">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="123">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="127">
+        <f>SUM(E27:M27)</f>
+        <v>994.3309999999999</v>
+      </c>
+      <c r="O27" s="127">
+        <f>N27*19.55%</f>
+        <v>194.39171049999999</v>
+      </c>
+      <c r="S27">
+        <f>(V27+90)/[2]calliope_2!$D$11</f>
+        <v>0.96517459253889637</v>
+      </c>
+      <c r="T27">
+        <v>0.93240000000000001</v>
+      </c>
+      <c r="U27" s="127">
+        <f>V27-[2]calliope_2!$L$2</f>
+        <v>-85.732250558458134</v>
+      </c>
+      <c r="V27" s="139">
+        <f>SUM(W3:AE8)</f>
+        <v>267.21926999999999</v>
+      </c>
+      <c r="W27" s="123">
+        <f t="shared" ref="W27:AE27" si="15">SUM(W3:W8)</f>
+        <v>5.55</v>
+      </c>
+      <c r="X27" s="123">
+        <f t="shared" si="15"/>
+        <v>204.92</v>
+      </c>
+      <c r="Y27" s="123">
+        <f t="shared" si="15"/>
+        <v>18.700000000000003</v>
+      </c>
+      <c r="Z27" s="123">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="123">
+        <f t="shared" si="15"/>
+        <v>2.7722500000000001</v>
+      </c>
+      <c r="AB27" s="123">
+        <f t="shared" si="15"/>
+        <v>35.097020000000001</v>
+      </c>
+      <c r="AC27" s="123">
+        <f t="shared" si="15"/>
+        <v>0.18</v>
+      </c>
+      <c r="AD27" s="123">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE27" s="123">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF27" s="123">
+        <f t="shared" ref="AF27" si="16">SUM(AF3:AF8)</f>
+        <v>90</v>
+      </c>
+      <c r="AG27" s="138"/>
+      <c r="AH27" s="138"/>
+      <c r="AI27" s="138"/>
+      <c r="AJ27" s="138"/>
+      <c r="AK27" s="138"/>
+      <c r="AL27" s="138"/>
+      <c r="AM27" s="138"/>
+      <c r="AN27" s="138"/>
+      <c r="AO27" s="138"/>
+      <c r="AP27" s="138"/>
+      <c r="AQ27" s="138"/>
+      <c r="AR27" s="138"/>
+      <c r="AS27" s="138"/>
+      <c r="AT27" s="138"/>
+      <c r="AU27" s="138"/>
+      <c r="AV27" s="138"/>
+      <c r="AW27" s="138"/>
+      <c r="AX27" s="138"/>
+      <c r="AY27" s="138"/>
+    </row>
+    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="C28" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="135"/>
+      <c r="E28" s="123">
+        <f>SUM(E9:E16)</f>
+        <v>19.799999999999997</v>
+      </c>
+      <c r="F28" s="123">
+        <f t="shared" ref="F28:M28" si="17">SUM(F9:F16)</f>
+        <v>1031.268</v>
+      </c>
+      <c r="G28" s="123">
+        <f t="shared" si="17"/>
+        <v>156.304</v>
+      </c>
+      <c r="H28" s="123">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="123">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="J28" s="123">
+        <f t="shared" si="17"/>
+        <v>335.57500000000005</v>
+      </c>
+      <c r="K28" s="123">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="123">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="123">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="127">
+        <f t="shared" ref="N28:N29" si="18">SUM(E28:M28)</f>
+        <v>1572.9470000000001</v>
+      </c>
+      <c r="O28" s="127">
+        <f>N28*14.02%</f>
+        <v>220.52716939999999</v>
+      </c>
+      <c r="S28">
+        <f>SUM(V28:V29)/SUM([2]calliope_2!$E$11:$F$11)</f>
+        <v>1.210630155595751</v>
+      </c>
+      <c r="T28">
+        <v>0.95479999999999998</v>
+      </c>
+      <c r="U28" s="127">
+        <f>V28-(SUM([2]calliope_2!$M$2:$N$2))</f>
+        <v>80.152327944426588</v>
+      </c>
+      <c r="V28" s="139">
+        <f>SUMPRODUCT(W9:AE16)</f>
+        <v>619.59340999999995</v>
+      </c>
+      <c r="W28" s="123">
+        <f t="shared" ref="W28:AE28" si="19">SUM(W9:W16)</f>
+        <v>5.9399999999999995</v>
+      </c>
+      <c r="X28" s="123">
+        <f t="shared" si="19"/>
+        <v>484.69595999999996</v>
+      </c>
+      <c r="Y28" s="123">
+        <f t="shared" si="19"/>
+        <v>85.967200000000005</v>
+      </c>
+      <c r="Z28" s="123">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="123">
+        <f t="shared" si="19"/>
+        <v>19.5</v>
+      </c>
+      <c r="AB28" s="123">
+        <f t="shared" si="19"/>
+        <v>23.490250000000003</v>
+      </c>
+      <c r="AC28" s="123">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AD28" s="123">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="123">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AF28" s="123">
+        <f t="shared" ref="AF28" si="20">SUM(AF9:AF16)</f>
+        <v>0</v>
+      </c>
+      <c r="AG28" s="138"/>
+      <c r="AH28" s="138"/>
+      <c r="AI28" s="138"/>
+      <c r="AJ28" s="138"/>
+      <c r="AK28" s="138"/>
+      <c r="AL28" s="138"/>
+      <c r="AM28" s="138"/>
+      <c r="AN28" s="138"/>
+      <c r="AO28" s="138"/>
+      <c r="AP28" s="138"/>
+      <c r="AQ28" s="138"/>
+      <c r="AR28" s="138"/>
+      <c r="AS28" s="138"/>
+      <c r="AT28" s="138"/>
+      <c r="AU28" s="138"/>
+      <c r="AV28" s="138"/>
+      <c r="AW28" s="138"/>
+      <c r="AX28" s="138"/>
+      <c r="AY28" s="138"/>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="C29" s="120" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="135"/>
+      <c r="E29" s="123">
+        <f>SUM(E17:E22)</f>
+        <v>2.81</v>
+      </c>
+      <c r="F29" s="123">
+        <f t="shared" ref="F29:M29" si="21">SUM(F17:F22)</f>
+        <v>1018.63</v>
+      </c>
+      <c r="G29" s="123">
+        <f t="shared" si="21"/>
+        <v>319.93399999999997</v>
+      </c>
+      <c r="H29" s="123">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="123">
+        <f t="shared" si="21"/>
+        <v>0.24</v>
+      </c>
+      <c r="J29" s="123">
+        <f t="shared" si="21"/>
+        <v>735.56000000000006</v>
+      </c>
+      <c r="K29" s="123">
+        <f t="shared" si="21"/>
+        <v>1.04</v>
+      </c>
+      <c r="L29" s="123">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="123">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="127">
+        <f t="shared" si="18"/>
+        <v>2078.2139999999999</v>
+      </c>
+      <c r="O29" s="127">
+        <f>N29*31.62%</f>
+        <v>657.13126680000005</v>
+      </c>
+      <c r="T29">
+        <v>0.94810000000000005</v>
+      </c>
+      <c r="U29" s="127">
+        <f>V29-SUM([2]calliope_2!$O$2:$P$2)</f>
+        <v>199.21791289160831</v>
+      </c>
+      <c r="V29" s="139">
+        <f>SUMPRODUCT(W17:AE22)</f>
+        <v>708.24799999999993</v>
+      </c>
+      <c r="W29" s="123">
+        <f t="shared" ref="W29:AE29" si="22">SUM(W17:W22)</f>
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="X29" s="123">
+        <f t="shared" si="22"/>
+        <v>478.75609999999995</v>
+      </c>
+      <c r="Y29" s="123">
+        <f t="shared" si="22"/>
+        <v>175.96370000000002</v>
+      </c>
+      <c r="Z29" s="123">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="123">
+        <f t="shared" si="22"/>
+        <v>0.156</v>
+      </c>
+      <c r="AB29" s="123">
+        <f t="shared" si="22"/>
+        <v>51.489200000000004</v>
+      </c>
+      <c r="AC29" s="123">
+        <f t="shared" si="22"/>
+        <v>1.04</v>
+      </c>
+      <c r="AD29" s="123">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="123">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AF29" s="123">
+        <f t="shared" ref="AF29" si="23">SUM(AF17:AF22)</f>
+        <v>0</v>
+      </c>
+      <c r="AG29" s="138"/>
+      <c r="AH29" s="138"/>
+      <c r="AI29" s="138"/>
+      <c r="AJ29" s="138"/>
+      <c r="AK29" s="138"/>
+      <c r="AL29" s="138"/>
+      <c r="AM29" s="138"/>
+      <c r="AN29" s="138"/>
+      <c r="AO29" s="138"/>
+      <c r="AP29" s="138"/>
+      <c r="AQ29" s="138"/>
+      <c r="AR29" s="138"/>
+      <c r="AS29" s="138"/>
+      <c r="AT29" s="138"/>
+      <c r="AU29" s="138"/>
+      <c r="AV29" s="138"/>
+      <c r="AW29" s="138"/>
+      <c r="AX29" s="138"/>
+      <c r="AY29" s="138"/>
+    </row>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
       <c r="E30" s="123"/>
       <c r="F30" s="123"/>
       <c r="G30" s="123"/>
@@ -6211,8 +7494,22 @@
       <c r="K30" s="123"/>
       <c r="L30" s="123"/>
       <c r="M30" s="123"/>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="N30" s="127">
+        <f>SUM(N27:N29)</f>
+        <v>4645.4920000000002</v>
+      </c>
+      <c r="O30" s="127">
+        <f>SUM(O27:O29)</f>
+        <v>1072.0501466999999</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
       <c r="E31" s="123"/>
       <c r="F31" s="123"/>
       <c r="G31" s="123"/>
@@ -6222,8 +7519,12 @@
       <c r="K31" s="123"/>
       <c r="L31" s="123"/>
       <c r="M31" s="123"/>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AE31" s="137">
+        <v>6.82</v>
+      </c>
+      <c r="AF31" s="137"/>
+    </row>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
       <c r="E32" s="123"/>
       <c r="F32" s="123"/>
       <c r="G32" s="123"/>
@@ -6399,16 +7700,67 @@
       <c r="L47" s="123"/>
       <c r="M47" s="123"/>
     </row>
+    <row r="48" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E48" s="123"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="123"/>
+      <c r="H48" s="123"/>
+      <c r="I48" s="123"/>
+      <c r="J48" s="123"/>
+      <c r="K48" s="123"/>
+      <c r="L48" s="123"/>
+      <c r="M48" s="123"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E49" s="123"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="123"/>
+      <c r="H49" s="123"/>
+      <c r="I49" s="123"/>
+      <c r="J49" s="123"/>
+      <c r="K49" s="123"/>
+      <c r="L49" s="123"/>
+      <c r="M49" s="123"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E50" s="123"/>
+      <c r="F50" s="123"/>
+      <c r="G50" s="123"/>
+      <c r="H50" s="123"/>
+      <c r="I50" s="123"/>
+      <c r="J50" s="123"/>
+      <c r="K50" s="123"/>
+      <c r="L50" s="123"/>
+      <c r="M50" s="123"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E51" s="123"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="123"/>
+      <c r="H51" s="123"/>
+      <c r="I51" s="123"/>
+      <c r="J51" s="123"/>
+      <c r="K51" s="123"/>
+      <c r="L51" s="123"/>
+      <c r="M51" s="123"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="AP1:AX1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="N1:V1"/>
     <mergeCell ref="W1:AE1"/>
-    <mergeCell ref="AF1:AN1"/>
+    <mergeCell ref="AG1:AO1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6437,39 +7789,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130" t="s">
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="130"/>
-      <c r="W1" s="135" t="s">
+      <c r="O1" s="142"/>
+      <c r="P1" s="142"/>
+      <c r="Q1" s="142"/>
+      <c r="R1" s="142"/>
+      <c r="S1" s="142"/>
+      <c r="T1" s="142"/>
+      <c r="U1" s="142"/>
+      <c r="V1" s="142"/>
+      <c r="W1" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="135"/>
-      <c r="Y1" s="135"/>
-      <c r="Z1" s="135"/>
-      <c r="AA1" s="135"/>
-      <c r="AB1" s="135"/>
-      <c r="AC1" s="135"/>
-      <c r="AD1" s="135"/>
-      <c r="AE1" s="135"/>
+      <c r="X1" s="149"/>
+      <c r="Y1" s="149"/>
+      <c r="Z1" s="149"/>
+      <c r="AA1" s="149"/>
+      <c r="AB1" s="149"/>
+      <c r="AC1" s="149"/>
+      <c r="AD1" s="149"/>
+      <c r="AE1" s="149"/>
     </row>
     <row r="2" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -6570,7 +7922,7 @@
       <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="132">
+      <c r="D3" s="146">
         <v>1</v>
       </c>
       <c r="E3" s="83">
@@ -6662,7 +8014,7 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="133"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="85"/>
       <c r="F4" s="36"/>
       <c r="G4" s="37"/>
@@ -6695,7 +8047,7 @@
       <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="133"/>
+      <c r="D5" s="147"/>
       <c r="E5" s="85"/>
       <c r="F5" s="36"/>
       <c r="G5" s="37"/>
@@ -6728,7 +8080,7 @@
       <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="133"/>
+      <c r="D6" s="147"/>
       <c r="E6" s="85"/>
       <c r="F6" s="36"/>
       <c r="G6" s="37"/>
@@ -6761,7 +8113,7 @@
       <c r="C7" s="3">
         <v>4</v>
       </c>
-      <c r="D7" s="133"/>
+      <c r="D7" s="147"/>
       <c r="E7" s="85"/>
       <c r="F7" s="36"/>
       <c r="G7" s="37"/>
@@ -6794,7 +8146,7 @@
       <c r="C8" s="3">
         <v>5</v>
       </c>
-      <c r="D8" s="133"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="85"/>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
@@ -6827,7 +8179,7 @@
       <c r="C9" s="3">
         <v>11</v>
       </c>
-      <c r="D9" s="134"/>
+      <c r="D9" s="148"/>
       <c r="E9" s="87"/>
       <c r="F9" s="46"/>
       <c r="G9" s="47"/>
@@ -6860,7 +8212,7 @@
       <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="D10" s="132">
+      <c r="D10" s="146">
         <v>2</v>
       </c>
       <c r="E10" s="83">
@@ -6951,7 +8303,7 @@
       <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="134"/>
+      <c r="D11" s="148"/>
       <c r="E11" s="87"/>
       <c r="F11" s="46"/>
       <c r="G11" s="47"/>
@@ -6984,7 +8336,7 @@
       <c r="C12" s="1">
         <v>6</v>
       </c>
-      <c r="D12" s="132">
+      <c r="D12" s="146">
         <v>3</v>
       </c>
       <c r="E12" s="83">
@@ -7075,7 +8427,7 @@
       <c r="C13" s="1">
         <v>7</v>
       </c>
-      <c r="D13" s="133"/>
+      <c r="D13" s="147"/>
       <c r="E13" s="85"/>
       <c r="F13" s="36"/>
       <c r="G13" s="37"/>
@@ -7108,7 +8460,7 @@
       <c r="C14" s="1">
         <v>8</v>
       </c>
-      <c r="D14" s="134"/>
+      <c r="D14" s="148"/>
       <c r="E14" s="87"/>
       <c r="F14" s="46"/>
       <c r="G14" s="47"/>
@@ -7147,7 +8499,7 @@
       <c r="C15" s="6">
         <v>13</v>
       </c>
-      <c r="D15" s="132">
+      <c r="D15" s="146">
         <v>4</v>
       </c>
       <c r="E15" s="83">
@@ -7235,7 +8587,7 @@
       <c r="C16" s="6">
         <v>14</v>
       </c>
-      <c r="D16" s="133"/>
+      <c r="D16" s="147"/>
       <c r="E16" s="85"/>
       <c r="F16" s="36"/>
       <c r="G16" s="37"/>
@@ -7268,7 +8620,7 @@
       <c r="C17" s="6">
         <v>15</v>
       </c>
-      <c r="D17" s="134"/>
+      <c r="D17" s="148"/>
       <c r="E17" s="87"/>
       <c r="F17" s="46"/>
       <c r="G17" s="47"/>
@@ -7307,7 +8659,7 @@
       <c r="C18" s="7">
         <v>16</v>
       </c>
-      <c r="D18" s="132">
+      <c r="D18" s="146">
         <v>5</v>
       </c>
       <c r="E18" s="83"/>
@@ -7392,7 +8744,7 @@
       <c r="C19" s="7">
         <v>17</v>
       </c>
-      <c r="D19" s="133"/>
+      <c r="D19" s="147"/>
       <c r="E19" s="85"/>
       <c r="F19" s="36"/>
       <c r="G19" s="37"/>
@@ -7425,7 +8777,7 @@
       <c r="C20" s="7">
         <v>18</v>
       </c>
-      <c r="D20" s="133"/>
+      <c r="D20" s="147"/>
       <c r="E20" s="85"/>
       <c r="F20" s="36"/>
       <c r="G20" s="37"/>
@@ -7458,7 +8810,7 @@
       <c r="C21" s="7">
         <v>19</v>
       </c>
-      <c r="D21" s="133"/>
+      <c r="D21" s="147"/>
       <c r="E21" s="85"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -7491,7 +8843,7 @@
       <c r="C22" s="7">
         <v>20</v>
       </c>
-      <c r="D22" s="133"/>
+      <c r="D22" s="147"/>
       <c r="E22" s="85"/>
       <c r="F22" s="36"/>
       <c r="G22" s="37"/>
@@ -7524,7 +8876,7 @@
       <c r="C23" s="7">
         <v>21</v>
       </c>
-      <c r="D23" s="134"/>
+      <c r="D23" s="148"/>
       <c r="E23" s="87"/>
       <c r="F23" s="46"/>
       <c r="G23" s="47"/>
@@ -7563,7 +8915,7 @@
       <c r="C24" s="8">
         <v>36</v>
       </c>
-      <c r="D24" s="132">
+      <c r="D24" s="146">
         <v>7</v>
       </c>
       <c r="E24" s="83"/>
@@ -7652,7 +9004,7 @@
       <c r="C25" s="8">
         <v>37</v>
       </c>
-      <c r="D25" s="133"/>
+      <c r="D25" s="147"/>
       <c r="E25" s="85"/>
       <c r="F25" s="36"/>
       <c r="G25" s="37"/>
@@ -7685,7 +9037,7 @@
       <c r="C26" s="8">
         <v>38</v>
       </c>
-      <c r="D26" s="134"/>
+      <c r="D26" s="148"/>
       <c r="E26" s="87"/>
       <c r="F26" s="46"/>
       <c r="G26" s="47"/>
@@ -7815,7 +9167,7 @@
       <c r="C28" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="132">
+      <c r="D28" s="146">
         <v>8</v>
       </c>
       <c r="E28" s="83"/>
@@ -7902,7 +9254,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C29" s="17"/>
-      <c r="D29" s="133"/>
+      <c r="D29" s="147"/>
       <c r="E29" s="85"/>
       <c r="F29" s="36"/>
       <c r="G29" s="37"/>
@@ -7933,7 +9285,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C30" s="17"/>
-      <c r="D30" s="133"/>
+      <c r="D30" s="147"/>
       <c r="E30" s="85"/>
       <c r="F30" s="36"/>
       <c r="G30" s="37"/>
@@ -7964,7 +9316,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C31" s="17"/>
-      <c r="D31" s="133"/>
+      <c r="D31" s="147"/>
       <c r="E31" s="85"/>
       <c r="F31" s="36"/>
       <c r="G31" s="37"/>
@@ -7995,7 +9347,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C32" s="17"/>
-      <c r="D32" s="133"/>
+      <c r="D32" s="147"/>
       <c r="E32" s="85"/>
       <c r="F32" s="36"/>
       <c r="G32" s="37"/>
@@ -8026,7 +9378,7 @@
     </row>
     <row r="33" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="17"/>
-      <c r="D33" s="134"/>
+      <c r="D33" s="148"/>
       <c r="E33" s="87"/>
       <c r="F33" s="46"/>
       <c r="G33" s="47"/>
@@ -8065,7 +9417,7 @@
       <c r="C34" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="132">
+      <c r="D34" s="146">
         <v>9</v>
       </c>
       <c r="E34" s="83">
@@ -8154,7 +9506,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C35" s="25"/>
-      <c r="D35" s="133"/>
+      <c r="D35" s="147"/>
       <c r="E35" s="85"/>
       <c r="F35" s="36"/>
       <c r="G35" s="37"/>
@@ -8185,7 +9537,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C36" s="25"/>
-      <c r="D36" s="133"/>
+      <c r="D36" s="147"/>
       <c r="E36" s="85"/>
       <c r="F36" s="36"/>
       <c r="G36" s="37"/>
@@ -8216,7 +9568,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C37" s="25"/>
-      <c r="D37" s="133"/>
+      <c r="D37" s="147"/>
       <c r="E37" s="85"/>
       <c r="F37" s="36"/>
       <c r="G37" s="37"/>
@@ -8247,7 +9599,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C38" s="25"/>
-      <c r="D38" s="133"/>
+      <c r="D38" s="147"/>
       <c r="E38" s="85"/>
       <c r="F38" s="36"/>
       <c r="G38" s="37"/>
@@ -8278,7 +9630,7 @@
     </row>
     <row r="39" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39" s="25"/>
-      <c r="D39" s="134"/>
+      <c r="D39" s="148"/>
       <c r="E39" s="87"/>
       <c r="F39" s="46"/>
       <c r="G39" s="47"/>
@@ -9018,22 +10370,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="137" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="138" t="s">
+      <c r="B1" s="130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="138" t="s">
+      <c r="D1" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="138" t="s">
+      <c r="E1" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="138" t="s">
+      <c r="F1" s="131" t="s">
         <v>71</v>
       </c>
       <c r="G1" s="120"/>
@@ -9046,13 +10398,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="120"/>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="139">
+      <c r="C2" s="132">
         <v>2.5</v>
       </c>
-      <c r="D2" s="139">
+      <c r="D2" s="132">
         <v>3</v>
       </c>
       <c r="E2" s="120"/>
@@ -9070,13 +10422,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="120"/>
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="139">
+      <c r="C3" s="132">
         <v>1.65</v>
       </c>
-      <c r="D3" s="139">
+      <c r="D3" s="132">
         <v>0.13</v>
       </c>
       <c r="E3" s="120"/>
@@ -9093,13 +10445,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="120"/>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="139">
+      <c r="C4" s="132">
         <v>0.75</v>
       </c>
-      <c r="D4" s="139">
+      <c r="D4" s="132">
         <v>2</v>
       </c>
       <c r="E4" s="120"/>
@@ -9116,13 +10468,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="120"/>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="139">
+      <c r="C5" s="132">
         <v>4.5</v>
       </c>
-      <c r="D5" s="139">
+      <c r="D5" s="132">
         <v>0.5</v>
       </c>
       <c r="E5" s="120"/>
@@ -9139,13 +10491,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="120"/>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="139">
+      <c r="C6" s="132">
         <v>1.9</v>
       </c>
-      <c r="D6" s="139">
+      <c r="D6" s="132">
         <v>0.5</v>
       </c>
       <c r="E6" s="120"/>
@@ -9162,13 +10514,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="120"/>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="139">
+      <c r="C7" s="132">
         <v>1.2</v>
       </c>
-      <c r="D7" s="139">
+      <c r="D7" s="132">
         <v>3</v>
       </c>
       <c r="E7" s="120"/>
@@ -9185,13 +10537,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="120"/>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="139">
+      <c r="C8" s="132">
         <v>0.95</v>
       </c>
-      <c r="D8" s="139">
+      <c r="D8" s="132">
         <v>0.37</v>
       </c>
       <c r="E8" s="120"/>
@@ -9208,11 +10560,11 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="120"/>
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
       <c r="E9" s="120"/>
       <c r="F9" s="120"/>
       <c r="G9" s="120"/>
@@ -9225,13 +10577,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="120"/>
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="139">
+      <c r="C10" s="132">
         <v>1.88</v>
       </c>
-      <c r="D10" s="139">
+      <c r="D10" s="132">
         <v>0</v>
       </c>
       <c r="E10" s="120"/>
@@ -9248,13 +10600,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="120"/>
-      <c r="B11" s="140" t="s">
+      <c r="B11" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="139">
+      <c r="C11" s="132">
         <v>4</v>
       </c>
-      <c r="D11" s="139">
+      <c r="D11" s="132">
         <v>0</v>
       </c>
       <c r="E11" s="120"/>
@@ -9285,7 +10637,7 @@
       <c r="M12" s="120"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="130" t="s">
         <v>63</v>
       </c>
       <c r="B13" s="120"/>

</xml_diff>

<commit_message>
eighth update: done running the 2021 scenario
</commit_message>
<xml_diff>
--- a/database/calliope_generators.xlsx
+++ b/database/calliope_generators.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_power_system\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C328CC-C960-46FF-893D-7D3489E4A6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412CA925-12AC-47AA-9A98-B0CA24D61982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (3)" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="90">
   <si>
     <t>bus</t>
   </si>
@@ -241,16 +241,10 @@
     <t>slwahid</t>
   </si>
   <si>
-    <t>om_cost (USD/MWh)</t>
-  </si>
-  <si>
     <t>wind_ons</t>
   </si>
   <si>
     <t>wind_offs</t>
-  </si>
-  <si>
-    <t>cap_cost (USD/MW)</t>
   </si>
   <si>
     <t>lombok_energy_outlook</t>
@@ -296,6 +290,27 @@
   </si>
   <si>
     <t>electrification ratio</t>
+  </si>
+  <si>
+    <t>v_om_cost (USD/MWh)</t>
+  </si>
+  <si>
+    <t>fix_om_cost (kUSD/MW)</t>
+  </si>
+  <si>
+    <t>fische</t>
+  </si>
+  <si>
+    <t>nrel.gov</t>
+  </si>
+  <si>
+    <t>cap_cost (mUSD/MW)</t>
+  </si>
+  <si>
+    <t>iesr</t>
+  </si>
+  <si>
+    <t>ramp rate (min-1)</t>
   </si>
 </sst>
 </file>
@@ -883,10 +898,10 @@
       <xdr:rowOff>178592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>323467</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>327277</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>15715</xdr:rowOff>
+      <xdr:rowOff>19525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3370,20 +3385,21 @@
   <dimension ref="A1:AY56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BA14" sqref="BA14"/>
+      <selection pane="bottomRight" activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.109375" style="120" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="8.88671875" style="120" customWidth="1"/>
-    <col min="14" max="23" width="8.88671875" customWidth="1"/>
-    <col min="31" max="32" width="8.88671875" customWidth="1"/>
-    <col min="33" max="50" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="12" width="8.88671875" style="120" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="120" hidden="1" customWidth="1"/>
+    <col min="14" max="31" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="32" max="41" width="8.88671875" customWidth="1"/>
+    <col min="42" max="50" width="8.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">
@@ -3403,7 +3419,7 @@
       <c r="L1" s="144"/>
       <c r="M1" s="144"/>
       <c r="N1" s="142" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O1" s="142"/>
       <c r="P1" s="142"/>
@@ -3437,7 +3453,7 @@
       <c r="AN1" s="142"/>
       <c r="AO1" s="142"/>
       <c r="AP1" s="142" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AQ1" s="142"/>
       <c r="AR1" s="142"/>
@@ -3543,7 +3559,7 @@
         <v>9</v>
       </c>
       <c r="AF2" s="140" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AG2" s="101" t="s">
         <v>4</v>
@@ -7011,7 +7027,7 @@
       <c r="L25" s="123"/>
       <c r="M25" s="123"/>
       <c r="V25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W25" s="137">
         <v>0.52</v>
@@ -7075,13 +7091,13 @@
       <c r="L26" s="123"/>
       <c r="M26" s="123"/>
       <c r="T26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="V26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="W26" s="137"/>
       <c r="X26" s="137"/>
@@ -7115,7 +7131,7 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.3">
       <c r="C27" s="120" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="135"/>
       <c r="E27" s="123">
@@ -7239,7 +7255,7 @@
     </row>
     <row r="28" spans="1:51" x14ac:dyDescent="0.3">
       <c r="C28" s="120" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="135"/>
       <c r="E28" s="123">
@@ -7363,7 +7379,7 @@
     </row>
     <row r="29" spans="1:51" x14ac:dyDescent="0.3">
       <c r="C29" s="120" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="135"/>
       <c r="E29" s="123">
@@ -7503,12 +7519,12 @@
         <v>1072.0501466999999</v>
       </c>
       <c r="AE30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E31" s="123"/>
       <c r="F31" s="123"/>
@@ -7746,7 +7762,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -7765,6 +7781,535 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3A0967-938E-4AEF-B084-DA659F2B9109}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="131" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="131" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="131" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="131" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="131" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="120"/>
+      <c r="B2" s="129" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="132">
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="132">
+        <v>3</v>
+      </c>
+      <c r="E2" s="132">
+        <v>48</v>
+      </c>
+      <c r="F2" s="132">
+        <v>20</v>
+      </c>
+      <c r="G2" s="120">
+        <f>0.5*1000</f>
+        <v>500</v>
+      </c>
+      <c r="H2" s="132">
+        <v>0.04</v>
+      </c>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="120"/>
+      <c r="B3" s="129" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="132">
+        <v>1.65</v>
+      </c>
+      <c r="D3" s="132">
+        <v>0.13</v>
+      </c>
+      <c r="E3" s="132">
+        <v>45</v>
+      </c>
+      <c r="F3" s="132">
+        <v>40</v>
+      </c>
+      <c r="G3" s="120">
+        <v>849</v>
+      </c>
+      <c r="H3" s="132">
+        <v>0.01</v>
+      </c>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="120"/>
+      <c r="B4" s="129" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="132">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="132">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="132">
+        <v>23</v>
+      </c>
+      <c r="F4" s="132">
+        <v>30</v>
+      </c>
+      <c r="G4" s="120">
+        <v>433</v>
+      </c>
+      <c r="H4" s="132">
+        <v>0.12</v>
+      </c>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="120"/>
+      <c r="B5" s="129" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="132">
+        <v>4.5</v>
+      </c>
+      <c r="D5" s="132">
+        <v>0.37</v>
+      </c>
+      <c r="E5" s="132">
+        <v>20</v>
+      </c>
+      <c r="F5" s="132">
+        <v>30</v>
+      </c>
+      <c r="G5" s="120">
+        <v>38</v>
+      </c>
+      <c r="H5" s="132">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="120"/>
+      <c r="B6" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="132">
+        <v>1.9</v>
+      </c>
+      <c r="D6" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="132">
+        <v>53</v>
+      </c>
+      <c r="F6" s="132">
+        <v>80</v>
+      </c>
+      <c r="G6" s="120">
+        <v>6</v>
+      </c>
+      <c r="H6" s="132">
+        <v>0.3</v>
+      </c>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="120"/>
+      <c r="B7" s="129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="132">
+        <v>1.2</v>
+      </c>
+      <c r="D7" s="132">
+        <v>2.4</v>
+      </c>
+      <c r="E7" s="132">
+        <v>34.5</v>
+      </c>
+      <c r="F7" s="132">
+        <v>25</v>
+      </c>
+      <c r="G7" s="120">
+        <v>600</v>
+      </c>
+      <c r="H7" s="132">
+        <v>0.04</v>
+      </c>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="120"/>
+      <c r="B8" s="129" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="132">
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="132">
+        <v>0</v>
+      </c>
+      <c r="E8" s="132">
+        <v>15</v>
+      </c>
+      <c r="F8" s="132">
+        <v>25</v>
+      </c>
+      <c r="G8" s="120">
+        <v>7</v>
+      </c>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="120"/>
+      <c r="B9" s="129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="120"/>
+      <c r="B10" s="129" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="132">
+        <v>1.88</v>
+      </c>
+      <c r="D10" s="132">
+        <v>0</v>
+      </c>
+      <c r="E10" s="132">
+        <v>60</v>
+      </c>
+      <c r="F10" s="132">
+        <v>25</v>
+      </c>
+      <c r="G10" s="120">
+        <v>8</v>
+      </c>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="120"/>
+      <c r="B11" s="133" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="132">
+        <v>4</v>
+      </c>
+      <c r="D11" s="132">
+        <v>0</v>
+      </c>
+      <c r="E11" s="132">
+        <v>124</v>
+      </c>
+      <c r="F11" s="132">
+        <v>25</v>
+      </c>
+      <c r="G11" s="120">
+        <v>12</v>
+      </c>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="120"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="130" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="120"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="120" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="120" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="120" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="120"/>
+      <c r="M19" s="120"/>
+      <c r="N19" s="120"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="120"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="120"/>
+      <c r="F20" s="120"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="120"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="120"/>
+      <c r="K20" s="120"/>
+      <c r="L20" s="120"/>
+      <c r="M20" s="120"/>
+      <c r="N20" s="120"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="120"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
+      <c r="G21" s="120"/>
+      <c r="H21" s="120"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="120"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="120"/>
+      <c r="M21" s="120"/>
+      <c r="N21" s="120"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="120"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="120"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="120"/>
+      <c r="N22" s="120"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A63535-D95A-4D36-8C1E-9289FDA2D070}">
   <dimension ref="A1:AE93"/>
   <sheetViews>
@@ -10351,451 +10896,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3A0967-938E-4AEF-B084-DA659F2B9109}">
-  <dimension ref="A1:M22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="4" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="130" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="130" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="131" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="131" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="131" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="131" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="120"/>
-      <c r="B2" s="129" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="132">
-        <v>2.5</v>
-      </c>
-      <c r="D2" s="132">
-        <v>3</v>
-      </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120">
-        <f>0.5*1000</f>
-        <v>500</v>
-      </c>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="120"/>
-      <c r="B3" s="129" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="132">
-        <v>1.65</v>
-      </c>
-      <c r="D3" s="132">
-        <v>0.13</v>
-      </c>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120">
-        <v>849</v>
-      </c>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="129" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="132">
-        <v>0.75</v>
-      </c>
-      <c r="D4" s="132">
-        <v>2</v>
-      </c>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120">
-        <v>433</v>
-      </c>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="120"/>
-      <c r="B5" s="129" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="132">
-        <v>4.5</v>
-      </c>
-      <c r="D5" s="132">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120">
-        <v>38</v>
-      </c>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="129" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="132">
-        <v>1.9</v>
-      </c>
-      <c r="D6" s="132">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120">
-        <v>6</v>
-      </c>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="120"/>
-      <c r="B7" s="129" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="132">
-        <v>1.2</v>
-      </c>
-      <c r="D7" s="132">
-        <v>3</v>
-      </c>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120">
-        <v>600</v>
-      </c>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="120"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="129" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="132">
-        <v>0.95</v>
-      </c>
-      <c r="D8" s="132">
-        <v>0.37</v>
-      </c>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120">
-        <v>7</v>
-      </c>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="129" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="132">
-        <v>1.88</v>
-      </c>
-      <c r="D10" s="132">
-        <v>0</v>
-      </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120">
-        <v>8</v>
-      </c>
-      <c r="G10" s="120"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
-      <c r="B11" s="133" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="132">
-        <v>4</v>
-      </c>
-      <c r="D11" s="132">
-        <v>0</v>
-      </c>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120">
-        <v>12</v>
-      </c>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
-      <c r="B12" s="120"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="120"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="130" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
-      <c r="M13" s="120"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="120" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="120" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="120"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
-      <c r="M17" s="120"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="120"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="120"/>
-      <c r="B19" s="120"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="120"/>
-      <c r="K19" s="120"/>
-      <c r="L19" s="120"/>
-      <c r="M19" s="120"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="120"/>
-      <c r="B20" s="120"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="120"/>
-      <c r="K20" s="120"/>
-      <c r="L20" s="120"/>
-      <c r="M20" s="120"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="120"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="120"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="120"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="120"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="120"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Failed push via Git
</commit_message>
<xml_diff>
--- a/database/calliope_generators.xlsx
+++ b/database/calliope_generators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_power_system\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412CA925-12AC-47AA-9A98-B0CA24D61982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A37EA3-7C8E-44FF-A89B-B562416BF4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
+    <workbookView xWindow="11304" yWindow="24" windowWidth="11760" windowHeight="12360" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (3)" sheetId="3" r:id="rId1"/>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -864,6 +864,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3044,8 +3046,8 @@
       <sheetName val="-jr28gpurfjy0ufw0 (3)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="L2">
@@ -3076,10 +3078,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3382,13 +3384,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83E7F3-B837-43E6-BF88-00ED77709958}">
-  <dimension ref="A1:AY56"/>
+  <dimension ref="A1:BA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK7" sqref="AK7"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3402,7 +3404,7 @@
     <col min="42" max="50" width="8.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C1" s="143">
         <v>2021</v>
       </c>
@@ -3464,7 +3466,7 @@
       <c r="AW1" s="142"/>
       <c r="AX1" s="142"/>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3616,7 +3618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="126">
         <v>0.86423333300000005</v>
       </c>
@@ -3774,8 +3776,9 @@
       <c r="AX3" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA3" s="151"/>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="126">
         <v>4.5260000000000002E-2</v>
       </c>
@@ -3935,8 +3938,9 @@
       <c r="AX4" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA4" s="151"/>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="126">
         <v>1.1174249999999999</v>
       </c>
@@ -4099,8 +4103,9 @@
       <c r="AX5" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA5" s="151"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="126">
         <v>0.17745</v>
       </c>
@@ -4260,8 +4265,9 @@
       <c r="AX6" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA6" s="151"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="126">
         <v>6.3899999999999998E-2</v>
       </c>
@@ -4421,8 +4427,9 @@
       <c r="AX7" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA7" s="151"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="126">
         <v>-1.7742</v>
       </c>
@@ -4583,8 +4590,9 @@
       <c r="AX8" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA8" s="151"/>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="126">
         <v>-2.6152000000000002</v>
       </c>
@@ -4745,8 +4753,9 @@
       <c r="AX9" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA9" s="151"/>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="126">
         <v>-2.6220500000000002</v>
       </c>
@@ -4906,8 +4915,9 @@
       <c r="AX10" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA10" s="151"/>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A11" s="126">
         <v>-2.1166</v>
       </c>
@@ -5067,8 +5077,9 @@
       <c r="AX11" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA11" s="151"/>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A12" s="126">
         <v>-2.8550333330000002</v>
       </c>
@@ -5228,8 +5239,9 @@
       <c r="AX12" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA12" s="151"/>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A13" s="126">
         <v>-0.74419999999999997</v>
       </c>
@@ -5390,8 +5402,9 @@
       <c r="AX13" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA13" s="151"/>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A14" s="126">
         <v>-3.4291333329999998</v>
       </c>
@@ -5553,8 +5566,9 @@
       <c r="AX14" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA14" s="151"/>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A15" s="126">
         <v>-2.26065</v>
       </c>
@@ -5714,8 +5728,9 @@
       <c r="AX15" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="BA15" s="151"/>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A16" s="126">
         <v>-3.5974499999999998</v>
       </c>
@@ -5875,8 +5890,9 @@
       <c r="AX16" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA16" s="151"/>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A17" s="126">
         <v>-1.761425</v>
       </c>
@@ -6035,8 +6051,9 @@
       <c r="AX17" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA17" s="151"/>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A18" s="126">
         <v>-1.190416667</v>
       </c>
@@ -6197,8 +6214,9 @@
       <c r="AX18" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA18" s="151"/>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A19" s="126">
         <v>-0.48473333299999999</v>
       </c>
@@ -6360,8 +6378,9 @@
       <c r="AX19" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA19" s="151"/>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A20" s="126">
         <v>0.31574999999999998</v>
       </c>
@@ -6378,8 +6397,8 @@
         <v>0</v>
       </c>
       <c r="F20" s="111">
-        <f>'[1]Sheet 1'!$F$370+'[1]Sheet 1'!$F$371+'[1]Sheet 1'!$F$380+'[1]Sheet 1'!$F$385+'[1]Sheet 1'!$F$386</f>
-        <v>277.63</v>
+        <f>'[1]Sheet 1'!$F$370+'[1]Sheet 1'!$F$371+'[1]Sheet 1'!$F$380</f>
+        <v>259</v>
       </c>
       <c r="G20" s="112">
         <f>'[1]Sheet 1'!$F$372+'[1]Sheet 1'!$F$373+'[1]Sheet 1'!$F$374+'[1]Sheet 1'!$F$375+'[1]Sheet 1'!$F$376+'[1]Sheet 1'!$F$377+'[1]Sheet 1'!$F$379</f>
@@ -6437,7 +6456,7 @@
       </c>
       <c r="X20" s="111">
         <f t="shared" si="2"/>
-        <v>130.48609999999999</v>
+        <v>121.72999999999999</v>
       </c>
       <c r="Y20" s="112">
         <f t="shared" si="3"/>
@@ -6522,8 +6541,9 @@
       <c r="AX20" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA20" s="151"/>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A21" s="126">
         <v>1.0532999999999999</v>
       </c>
@@ -6541,8 +6561,8 @@
         <v>0.81</v>
       </c>
       <c r="F21" s="111">
-        <f>+'[1]Sheet 1'!$F$388+'[1]Sheet 1'!$F$405</f>
-        <v>39</v>
+        <f>+'[1]Sheet 1'!$F$388+'[1]Sheet 1'!$F$405+'[1]Sheet 1'!$F$385+'[1]Sheet 1'!$F$386</f>
+        <v>57.63</v>
       </c>
       <c r="G21" s="112">
         <v>0</v>
@@ -6599,7 +6619,7 @@
       </c>
       <c r="X21" s="111">
         <f t="shared" si="2"/>
-        <v>18.329999999999998</v>
+        <v>27.086099999999998</v>
       </c>
       <c r="Y21" s="112">
         <f t="shared" si="3"/>
@@ -6684,8 +6704,9 @@
       <c r="AX21" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA21" s="151"/>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A22" s="126">
         <v>3.2987666670000002</v>
       </c>
@@ -6848,8 +6869,9 @@
       <c r="AX22" s="118">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="BA22" s="151"/>
+    </row>
+    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C23" s="124" t="s">
         <v>60</v>
       </c>
@@ -6934,7 +6956,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D24" s="134">
         <f>SUM(W23:AE23)+AF5</f>
         <v>1685.0606800000003</v>
@@ -6944,7 +6966,9 @@
       <c r="G24" s="123"/>
       <c r="H24" s="123"/>
       <c r="I24" s="123"/>
-      <c r="J24" s="123"/>
+      <c r="J24" s="150">
+        <v>227.99</v>
+      </c>
       <c r="K24" s="123"/>
       <c r="L24" s="123"/>
       <c r="M24" s="123"/>
@@ -7012,7 +7036,7 @@
       <c r="AX24" s="120"/>
       <c r="AY24" s="120"/>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D25" s="135">
         <f>SUMPRODUCT(E3:M22,AG3:AO22)</f>
         <v>1424.3024999999996</v>
@@ -7022,7 +7046,10 @@
       <c r="G25" s="123"/>
       <c r="H25" s="123"/>
       <c r="I25" s="123"/>
-      <c r="J25" s="123"/>
+      <c r="J25" s="123">
+        <f>J24/J23</f>
+        <v>0.1449837553838709</v>
+      </c>
       <c r="K25" s="123"/>
       <c r="L25" s="123"/>
       <c r="M25" s="123"/>
@@ -7079,14 +7106,17 @@
       <c r="AX25" s="138"/>
       <c r="AY25" s="138"/>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D26" s="135"/>
       <c r="E26" s="123"/>
       <c r="F26" s="123"/>
       <c r="G26" s="123"/>
       <c r="H26" s="123"/>
       <c r="I26" s="123"/>
-      <c r="J26" s="123"/>
+      <c r="J26" s="123">
+        <f>J24-J23</f>
+        <v>-1344.5309999999997</v>
+      </c>
       <c r="K26" s="123"/>
       <c r="L26" s="123"/>
       <c r="M26" s="123"/>
@@ -7129,7 +7159,7 @@
       <c r="AX26" s="138"/>
       <c r="AY26" s="138"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C27" s="120" t="s">
         <v>75</v>
       </c>
@@ -7253,7 +7283,7 @@
       <c r="AX27" s="138"/>
       <c r="AY27" s="138"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C28" s="120" t="s">
         <v>76</v>
       </c>
@@ -7377,7 +7407,7 @@
       <c r="AX28" s="138"/>
       <c r="AY28" s="138"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C29" s="120" t="s">
         <v>77</v>
       </c>
@@ -7443,7 +7473,7 @@
       </c>
       <c r="X29" s="123">
         <f t="shared" si="22"/>
-        <v>478.75609999999995</v>
+        <v>478.7561</v>
       </c>
       <c r="Y29" s="123">
         <f t="shared" si="22"/>
@@ -7497,7 +7527,7 @@
       <c r="AX29" s="138"/>
       <c r="AY29" s="138"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -7522,7 +7552,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -7540,7 +7570,7 @@
       </c>
       <c r="AF31" s="137"/>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.3">
       <c r="E32" s="123"/>
       <c r="F32" s="123"/>
       <c r="G32" s="123"/>
@@ -7785,7 +7815,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7987,13 +8017,14 @@
         <v>7</v>
       </c>
       <c r="C7" s="132">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="132">
         <v>2.4</v>
       </c>
       <c r="E7" s="132">
-        <v>34.5</v>
+        <f>0.02*1000</f>
+        <v>20</v>
       </c>
       <c r="F7" s="132">
         <v>25</v>

</xml_diff>

<commit_message>
eleventh update: validated results of 2021 scenario
</commit_message>
<xml_diff>
--- a/database/calliope_generators.xlsx
+++ b/database/calliope_generators.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_power_system\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_energy_transition\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A37EA3-7C8E-44FF-A89B-B562416BF4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA99FDD1-F6E6-4855-97C9-2190CC195F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11304" yWindow="24" windowWidth="11760" windowHeight="12360" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
+    <workbookView xWindow="11244" yWindow="24" windowWidth="11892" windowHeight="8880" activeTab="1" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="esdm" sheetId="3" r:id="rId2"/>
+    <sheet name="ruptl" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
   <si>
     <t>bus</t>
   </si>
@@ -311,6 +312,9 @@
   </si>
   <si>
     <t>ramp rate (min-1)</t>
+  </si>
+  <si>
+    <t>diesel</t>
   </si>
 </sst>
 </file>
@@ -621,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -840,6 +844,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="17" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,8 +870,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3383,6 +3393,536 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3A0967-938E-4AEF-B084-DA659F2B9109}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="131" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="131" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="131" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="131" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="131" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="131" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="120"/>
+      <c r="B2" s="129" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="132">
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="132">
+        <v>3</v>
+      </c>
+      <c r="E2" s="132">
+        <v>48</v>
+      </c>
+      <c r="F2" s="132">
+        <v>20</v>
+      </c>
+      <c r="G2" s="120">
+        <f>0.5*1000</f>
+        <v>500</v>
+      </c>
+      <c r="H2" s="132">
+        <v>0.04</v>
+      </c>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="120"/>
+      <c r="B3" s="129" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="132">
+        <v>1.65</v>
+      </c>
+      <c r="D3" s="132">
+        <v>0.13</v>
+      </c>
+      <c r="E3" s="132">
+        <v>45</v>
+      </c>
+      <c r="F3" s="132">
+        <v>40</v>
+      </c>
+      <c r="G3" s="120">
+        <v>849</v>
+      </c>
+      <c r="H3" s="132">
+        <v>0.01</v>
+      </c>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="120"/>
+      <c r="B4" s="129" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="132">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="132">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="132">
+        <v>23</v>
+      </c>
+      <c r="F4" s="132">
+        <v>30</v>
+      </c>
+      <c r="G4" s="120">
+        <v>433</v>
+      </c>
+      <c r="H4" s="132">
+        <v>0.12</v>
+      </c>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="120"/>
+      <c r="B5" s="129" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="132">
+        <v>4.5</v>
+      </c>
+      <c r="D5" s="132">
+        <v>0.37</v>
+      </c>
+      <c r="E5" s="132">
+        <v>20</v>
+      </c>
+      <c r="F5" s="132">
+        <v>30</v>
+      </c>
+      <c r="G5" s="120">
+        <v>38</v>
+      </c>
+      <c r="H5" s="132">
+        <v>0.2</v>
+      </c>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="120"/>
+      <c r="B6" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="132">
+        <v>1.9</v>
+      </c>
+      <c r="D6" s="132">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="132">
+        <v>53</v>
+      </c>
+      <c r="F6" s="132">
+        <v>80</v>
+      </c>
+      <c r="G6" s="120">
+        <v>6</v>
+      </c>
+      <c r="H6" s="132">
+        <v>0.3</v>
+      </c>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="120"/>
+      <c r="B7" s="129" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="132">
+        <v>1</v>
+      </c>
+      <c r="D7" s="132">
+        <v>2.4</v>
+      </c>
+      <c r="E7" s="132">
+        <f>0.02*1000</f>
+        <v>20</v>
+      </c>
+      <c r="F7" s="132">
+        <v>25</v>
+      </c>
+      <c r="G7" s="120">
+        <v>600</v>
+      </c>
+      <c r="H7" s="132">
+        <v>0.04</v>
+      </c>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="120"/>
+      <c r="B8" s="129" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="132">
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="132">
+        <v>0</v>
+      </c>
+      <c r="E8" s="132">
+        <v>15</v>
+      </c>
+      <c r="F8" s="132">
+        <v>25</v>
+      </c>
+      <c r="G8" s="120">
+        <v>7</v>
+      </c>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="120"/>
+      <c r="B9" s="129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="120"/>
+      <c r="B10" s="129" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="132">
+        <v>1.88</v>
+      </c>
+      <c r="D10" s="132">
+        <v>0</v>
+      </c>
+      <c r="E10" s="132">
+        <v>60</v>
+      </c>
+      <c r="F10" s="132">
+        <v>25</v>
+      </c>
+      <c r="G10" s="120">
+        <v>8</v>
+      </c>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="120"/>
+      <c r="B11" s="133" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="132">
+        <v>4</v>
+      </c>
+      <c r="D11" s="132">
+        <v>0</v>
+      </c>
+      <c r="E11" s="132">
+        <v>124</v>
+      </c>
+      <c r="F11" s="132">
+        <v>25</v>
+      </c>
+      <c r="G11" s="120">
+        <v>12</v>
+      </c>
+      <c r="H11" s="120"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="120"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="120"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="120"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="130" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="120"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="120" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="120" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
+      <c r="F17" s="120"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="120" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="120" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="120"/>
+      <c r="M19" s="120"/>
+      <c r="N19" s="120"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="120"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="120"/>
+      <c r="F20" s="120"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="120"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="120"/>
+      <c r="K20" s="120"/>
+      <c r="L20" s="120"/>
+      <c r="M20" s="120"/>
+      <c r="N20" s="120"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="120"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
+      <c r="G21" s="120"/>
+      <c r="H21" s="120"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="120"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="120"/>
+      <c r="M21" s="120"/>
+      <c r="N21" s="120"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="120"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="120"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="120"/>
+      <c r="N22" s="120"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83E7F3-B837-43E6-BF88-00ED77709958}">
   <dimension ref="A1:BA56"/>
   <sheetViews>
@@ -3390,7 +3930,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3405,66 +3945,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="C1" s="143">
+      <c r="C1" s="145">
         <v>2021</v>
       </c>
-      <c r="D1" s="143"/>
-      <c r="E1" s="144" t="s">
+      <c r="D1" s="145"/>
+      <c r="E1" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="142" t="s">
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="144" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="142"/>
-      <c r="P1" s="142"/>
-      <c r="Q1" s="142"/>
-      <c r="R1" s="142"/>
-      <c r="S1" s="142"/>
-      <c r="T1" s="142"/>
-      <c r="U1" s="142"/>
-      <c r="V1" s="142"/>
-      <c r="W1" s="145" t="s">
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="144"/>
+      <c r="R1" s="144"/>
+      <c r="S1" s="144"/>
+      <c r="T1" s="144"/>
+      <c r="U1" s="144"/>
+      <c r="V1" s="144"/>
+      <c r="W1" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="145"/>
-      <c r="Y1" s="145"/>
-      <c r="Z1" s="145"/>
-      <c r="AA1" s="145"/>
-      <c r="AB1" s="145"/>
-      <c r="AC1" s="145"/>
-      <c r="AD1" s="145"/>
-      <c r="AE1" s="145"/>
+      <c r="X1" s="147"/>
+      <c r="Y1" s="147"/>
+      <c r="Z1" s="147"/>
+      <c r="AA1" s="147"/>
+      <c r="AB1" s="147"/>
+      <c r="AC1" s="147"/>
+      <c r="AD1" s="147"/>
+      <c r="AE1" s="147"/>
       <c r="AF1" s="128"/>
-      <c r="AG1" s="142" t="s">
+      <c r="AG1" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="142"/>
-      <c r="AI1" s="142"/>
-      <c r="AJ1" s="142"/>
-      <c r="AK1" s="142"/>
-      <c r="AL1" s="142"/>
-      <c r="AM1" s="142"/>
-      <c r="AN1" s="142"/>
-      <c r="AO1" s="142"/>
-      <c r="AP1" s="142" t="s">
+      <c r="AH1" s="144"/>
+      <c r="AI1" s="144"/>
+      <c r="AJ1" s="144"/>
+      <c r="AK1" s="144"/>
+      <c r="AL1" s="144"/>
+      <c r="AM1" s="144"/>
+      <c r="AN1" s="144"/>
+      <c r="AO1" s="144"/>
+      <c r="AP1" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="AQ1" s="142"/>
-      <c r="AR1" s="142"/>
-      <c r="AS1" s="142"/>
-      <c r="AT1" s="142"/>
-      <c r="AU1" s="142"/>
-      <c r="AV1" s="142"/>
-      <c r="AW1" s="142"/>
-      <c r="AX1" s="142"/>
+      <c r="AQ1" s="144"/>
+      <c r="AR1" s="144"/>
+      <c r="AS1" s="144"/>
+      <c r="AT1" s="144"/>
+      <c r="AU1" s="144"/>
+      <c r="AV1" s="144"/>
+      <c r="AW1" s="144"/>
+      <c r="AX1" s="144"/>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3776,7 +4316,7 @@
       <c r="AX3" s="118">
         <v>1</v>
       </c>
-      <c r="BA3" s="151"/>
+      <c r="BA3" s="143"/>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="126">
@@ -3938,7 +4478,7 @@
       <c r="AX4" s="118">
         <v>1</v>
       </c>
-      <c r="BA4" s="151"/>
+      <c r="BA4" s="143"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="126">
@@ -4103,7 +4643,7 @@
       <c r="AX5" s="118">
         <v>1</v>
       </c>
-      <c r="BA5" s="151"/>
+      <c r="BA5" s="143"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="126">
@@ -4119,14 +4659,14 @@
         <v>24</v>
       </c>
       <c r="E6" s="110">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6" s="111">
         <f>'[1]Sheet 1'!$F$89+'[1]Sheet 1'!$F$90+'[1]Sheet 1'!$F$91</f>
         <v>27</v>
       </c>
       <c r="G6" s="112">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H6" s="113">
         <v>0</v>
@@ -4177,7 +4717,7 @@
       </c>
       <c r="W6" s="110">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="X6" s="111">
         <f t="shared" si="2"/>
@@ -4185,7 +4725,7 @@
       </c>
       <c r="Y6" s="112">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>18.700000000000003</v>
       </c>
       <c r="Z6" s="113">
         <f t="shared" si="4"/>
@@ -4265,7 +4805,7 @@
       <c r="AX6" s="118">
         <v>1</v>
       </c>
-      <c r="BA6" s="151"/>
+      <c r="BA6" s="143"/>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="126">
@@ -4281,21 +4821,20 @@
         <v>26</v>
       </c>
       <c r="E7" s="110">
-        <f>'[1]Sheet 1'!$F$25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F7" s="111">
         <v>0</v>
       </c>
       <c r="G7" s="112">
-        <f>'[1]Sheet 1'!$F$19</f>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="H7" s="113">
         <v>0</v>
       </c>
       <c r="I7" s="114">
-        <v>0</v>
+        <f>'[1]Sheet 1'!$F$31+'[1]Sheet 1'!$F$32+'[1]Sheet 1'!$F$34+'[1]Sheet 1'!$F$55+'[1]Sheet 1'!$F$111</f>
+        <v>3.9650000000000003</v>
       </c>
       <c r="J7" s="115">
         <v>166.49600000000001</v>
@@ -4338,7 +4877,7 @@
       </c>
       <c r="W7" s="110">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="X7" s="111">
         <f t="shared" si="2"/>
@@ -4346,7 +4885,7 @@
       </c>
       <c r="Y7" s="112">
         <f t="shared" si="3"/>
-        <v>18.700000000000003</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="113">
         <f t="shared" si="4"/>
@@ -4354,7 +4893,7 @@
       </c>
       <c r="AA7" s="114">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.5772500000000003</v>
       </c>
       <c r="AB7" s="115">
         <f t="shared" si="6"/>
@@ -4427,7 +4966,7 @@
       <c r="AX7" s="118">
         <v>1</v>
       </c>
-      <c r="BA7" s="151"/>
+      <c r="BA7" s="143"/>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="126">
@@ -4590,7 +5129,7 @@
       <c r="AX8" s="118">
         <v>1</v>
       </c>
-      <c r="BA8" s="151"/>
+      <c r="BA8" s="143"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="126">
@@ -4753,7 +5292,7 @@
       <c r="AX9" s="118">
         <v>1</v>
       </c>
-      <c r="BA9" s="151"/>
+      <c r="BA9" s="143"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="126">
@@ -4915,7 +5454,7 @@
       <c r="AX10" s="118">
         <v>1</v>
       </c>
-      <c r="BA10" s="151"/>
+      <c r="BA10" s="143"/>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A11" s="126">
@@ -5077,7 +5616,7 @@
       <c r="AX11" s="118">
         <v>1</v>
       </c>
-      <c r="BA11" s="151"/>
+      <c r="BA11" s="143"/>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A12" s="126">
@@ -5239,7 +5778,7 @@
       <c r="AX12" s="118">
         <v>1</v>
       </c>
-      <c r="BA12" s="151"/>
+      <c r="BA12" s="143"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A13" s="126">
@@ -5402,7 +5941,7 @@
       <c r="AX13" s="118">
         <v>1</v>
       </c>
-      <c r="BA13" s="151"/>
+      <c r="BA13" s="143"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A14" s="126">
@@ -5566,7 +6105,7 @@
       <c r="AX14" s="118">
         <v>1</v>
       </c>
-      <c r="BA14" s="151"/>
+      <c r="BA14" s="143"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A15" s="126">
@@ -5728,7 +6267,7 @@
       <c r="AX15" s="118">
         <v>1</v>
       </c>
-      <c r="BA15" s="151"/>
+      <c r="BA15" s="143"/>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A16" s="126">
@@ -5890,7 +6429,7 @@
       <c r="AX16" s="118">
         <v>1</v>
       </c>
-      <c r="BA16" s="151"/>
+      <c r="BA16" s="143"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A17" s="126">
@@ -6051,7 +6590,7 @@
       <c r="AX17" s="118">
         <v>1</v>
       </c>
-      <c r="BA17" s="151"/>
+      <c r="BA17" s="143"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A18" s="126">
@@ -6214,7 +6753,7 @@
       <c r="AX18" s="118">
         <v>1</v>
       </c>
-      <c r="BA18" s="151"/>
+      <c r="BA18" s="143"/>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A19" s="126">
@@ -6378,7 +6917,7 @@
       <c r="AX19" s="118">
         <v>1</v>
       </c>
-      <c r="BA19" s="151"/>
+      <c r="BA19" s="143"/>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A20" s="126">
@@ -6541,7 +7080,7 @@
       <c r="AX20" s="118">
         <v>1</v>
       </c>
-      <c r="BA20" s="151"/>
+      <c r="BA20" s="143"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A21" s="126">
@@ -6704,7 +7243,7 @@
       <c r="AX21" s="118">
         <v>1</v>
       </c>
-      <c r="BA21" s="151"/>
+      <c r="BA21" s="143"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A22" s="126">
@@ -6869,7 +7408,7 @@
       <c r="AX22" s="118">
         <v>1</v>
       </c>
-      <c r="BA22" s="151"/>
+      <c r="BA22" s="143"/>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="C23" s="124" t="s">
@@ -6877,7 +7416,7 @@
       </c>
       <c r="D23" s="125">
         <f>SUM(E23:M23)</f>
-        <v>4645.4920000000002</v>
+        <v>4649.4569999999994</v>
       </c>
       <c r="E23" s="123">
         <f>SUM(E3:E22)</f>
@@ -6897,7 +7436,7 @@
       </c>
       <c r="I23" s="123">
         <f t="shared" si="10"/>
-        <v>34.505000000000003</v>
+        <v>38.470000000000006</v>
       </c>
       <c r="J23" s="123">
         <f t="shared" si="10"/>
@@ -6933,7 +7472,7 @@
       </c>
       <c r="AA23" s="127">
         <f t="shared" si="11"/>
-        <v>22.428249999999998</v>
+        <v>25.005499999999998</v>
       </c>
       <c r="AB23" s="127">
         <f t="shared" si="11"/>
@@ -6959,14 +7498,14 @@
     <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D24" s="134">
         <f>SUM(W23:AE23)+AF5</f>
-        <v>1685.0606800000003</v>
+        <v>1687.6379300000003</v>
       </c>
       <c r="E24" s="123"/>
       <c r="F24" s="123"/>
       <c r="G24" s="123"/>
       <c r="H24" s="123"/>
       <c r="I24" s="123"/>
-      <c r="J24" s="150">
+      <c r="J24" s="142">
         <v>227.99</v>
       </c>
       <c r="K24" s="123"/>
@@ -6978,15 +7517,15 @@
       </c>
       <c r="W24" s="136">
         <f>W23/$D$24*100</f>
-        <v>0.73190242620817658</v>
+        <v>0.73078471280862933</v>
       </c>
       <c r="X24" s="136">
         <f t="shared" ref="X24:AF24" si="13">X23/$D$24*100</f>
-        <v>69.337091172289405</v>
+        <v>69.231204112602512</v>
       </c>
       <c r="Y24" s="136">
         <f t="shared" si="13"/>
-        <v>16.654053075406161</v>
+        <v>16.62862009743997</v>
       </c>
       <c r="Z24" s="136">
         <f t="shared" si="13"/>
@@ -6994,15 +7533,15 @@
       </c>
       <c r="AA24" s="136">
         <f t="shared" si="13"/>
-        <v>1.3310054804673261</v>
+        <v>1.4816862998569837</v>
       </c>
       <c r="AB24" s="136">
         <f t="shared" si="13"/>
-        <v>6.5324929426280347</v>
+        <v>6.5225169476962384</v>
       </c>
       <c r="AC24" s="136">
         <f t="shared" si="13"/>
-        <v>7.2400953537174684E-2</v>
+        <v>7.2290387547760307E-2</v>
       </c>
       <c r="AD24" s="136">
         <f t="shared" si="13"/>
@@ -7014,7 +7553,7 @@
       </c>
       <c r="AF24" s="136">
         <f t="shared" si="13"/>
-        <v>5.3410539494637064</v>
+        <v>5.3328974420478907</v>
       </c>
       <c r="AG24" s="120"/>
       <c r="AH24" s="120"/>
@@ -7039,7 +7578,7 @@
     <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="D25" s="135">
         <f>SUMPRODUCT(E3:M22,AG3:AO22)</f>
-        <v>1424.3024999999996</v>
+        <v>1425.6109499999995</v>
       </c>
       <c r="E25" s="123"/>
       <c r="F25" s="123"/>
@@ -7163,7 +7702,10 @@
       <c r="C27" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="135"/>
+      <c r="D27" s="152">
+        <f>SUM(E27:L27)+AF27</f>
+        <v>1088.2959999999998</v>
+      </c>
       <c r="E27" s="123">
         <f>SUM(E3:E8)</f>
         <v>18.5</v>
@@ -7182,7 +7724,7 @@
       </c>
       <c r="I27" s="123">
         <f t="shared" si="14"/>
-        <v>4.2650000000000006</v>
+        <v>8.23</v>
       </c>
       <c r="J27" s="123">
         <f t="shared" si="14"/>
@@ -7202,26 +7744,26 @@
       </c>
       <c r="N27" s="127">
         <f>SUM(E27:M27)</f>
-        <v>994.3309999999999</v>
+        <v>998.29599999999994</v>
       </c>
       <c r="O27" s="127">
         <f>N27*19.55%</f>
-        <v>194.39171049999999</v>
+        <v>195.16686799999999</v>
       </c>
       <c r="S27">
         <f>(V27+90)/[2]calliope_2!$D$11</f>
-        <v>0.96517459253889637</v>
+        <v>0.97213809206852952</v>
       </c>
       <c r="T27">
         <v>0.93240000000000001</v>
       </c>
       <c r="U27" s="127">
         <f>V27-[2]calliope_2!$L$2</f>
-        <v>-85.732250558458134</v>
+        <v>-83.155000558458141</v>
       </c>
       <c r="V27" s="139">
         <f>SUM(W3:AE8)</f>
-        <v>267.21926999999999</v>
+        <v>269.79651999999999</v>
       </c>
       <c r="W27" s="123">
         <f t="shared" ref="W27:AE27" si="15">SUM(W3:W8)</f>
@@ -7241,7 +7783,7 @@
       </c>
       <c r="AA27" s="123">
         <f t="shared" si="15"/>
-        <v>2.7722500000000001</v>
+        <v>5.3495000000000008</v>
       </c>
       <c r="AB27" s="123">
         <f t="shared" si="15"/>
@@ -7287,45 +7829,48 @@
       <c r="C28" s="120" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="135"/>
+      <c r="D28" s="152">
+        <f t="shared" ref="D28:D29" si="17">SUM(E28:L28)+AF28</f>
+        <v>1572.9470000000001</v>
+      </c>
       <c r="E28" s="123">
         <f>SUM(E9:E16)</f>
         <v>19.799999999999997</v>
       </c>
       <c r="F28" s="123">
-        <f t="shared" ref="F28:M28" si="17">SUM(F9:F16)</f>
+        <f t="shared" ref="F28:M28" si="18">SUM(F9:F16)</f>
         <v>1031.268</v>
       </c>
       <c r="G28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>156.304</v>
       </c>
       <c r="H28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="I28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
       <c r="J28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>335.57500000000005</v>
       </c>
       <c r="K28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M28" s="123">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N28" s="127">
-        <f t="shared" ref="N28:N29" si="18">SUM(E28:M28)</f>
+        <f t="shared" ref="N28:N29" si="19">SUM(E28:M28)</f>
         <v>1572.9470000000001</v>
       </c>
       <c r="O28" s="127">
@@ -7348,43 +7893,43 @@
         <v>619.59340999999995</v>
       </c>
       <c r="W28" s="123">
-        <f t="shared" ref="W28:AE28" si="19">SUM(W9:W16)</f>
+        <f t="shared" ref="W28:AE28" si="20">SUM(W9:W16)</f>
         <v>5.9399999999999995</v>
       </c>
       <c r="X28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>484.69595999999996</v>
       </c>
       <c r="Y28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>85.967200000000005</v>
       </c>
       <c r="Z28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AA28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>19.5</v>
       </c>
       <c r="AB28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>23.490250000000003</v>
       </c>
       <c r="AC28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AD28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AE28" s="123">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AF28" s="123">
-        <f t="shared" ref="AF28" si="20">SUM(AF9:AF16)</f>
+        <f t="shared" ref="AF28" si="21">SUM(AF9:AF16)</f>
         <v>0</v>
       </c>
       <c r="AG28" s="138"/>
@@ -7411,45 +7956,48 @@
       <c r="C29" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="135"/>
+      <c r="D29" s="152">
+        <f t="shared" si="17"/>
+        <v>2078.2139999999999</v>
+      </c>
       <c r="E29" s="123">
         <f>SUM(E17:E22)</f>
         <v>2.81</v>
       </c>
       <c r="F29" s="123">
-        <f t="shared" ref="F29:M29" si="21">SUM(F17:F22)</f>
+        <f t="shared" ref="F29:M29" si="22">SUM(F17:F22)</f>
         <v>1018.63</v>
       </c>
       <c r="G29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>319.93399999999997</v>
       </c>
       <c r="H29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.24</v>
       </c>
       <c r="J29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>735.56000000000006</v>
       </c>
       <c r="K29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1.04</v>
       </c>
       <c r="L29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M29" s="123">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N29" s="127">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2078.2139999999999</v>
       </c>
       <c r="O29" s="127">
@@ -7468,43 +8016,43 @@
         <v>708.24799999999993</v>
       </c>
       <c r="W29" s="123">
-        <f t="shared" ref="W29:AE29" si="22">SUM(W17:W22)</f>
+        <f t="shared" ref="W29:AE29" si="23">SUM(W17:W22)</f>
         <v>0.84299999999999997</v>
       </c>
       <c r="X29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>478.7561</v>
       </c>
       <c r="Y29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>175.96370000000002</v>
       </c>
       <c r="Z29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AA29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.156</v>
       </c>
       <c r="AB29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>51.489200000000004</v>
       </c>
       <c r="AC29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.04</v>
       </c>
       <c r="AD29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AE29" s="123">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF29" s="123">
-        <f t="shared" ref="AF29" si="23">SUM(AF17:AF22)</f>
+        <f t="shared" ref="AF29" si="24">SUM(AF17:AF22)</f>
         <v>0</v>
       </c>
       <c r="AG29" s="138"/>
@@ -7531,6 +8079,7 @@
       <c r="A30" t="s">
         <v>63</v>
       </c>
+      <c r="D30" s="153"/>
       <c r="E30" s="123"/>
       <c r="F30" s="123"/>
       <c r="G30" s="123"/>
@@ -7542,11 +8091,11 @@
       <c r="M30" s="123"/>
       <c r="N30" s="127">
         <f>SUM(N27:N29)</f>
-        <v>4645.4920000000002</v>
+        <v>4649.4570000000003</v>
       </c>
       <c r="O30" s="127">
         <f>SUM(O27:O29)</f>
-        <v>1072.0501466999999</v>
+        <v>1072.8253042000001</v>
       </c>
       <c r="AE30" t="s">
         <v>74</v>
@@ -7810,537 +8359,671 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3A0967-938E-4AEF-B084-DA659F2B9109}">
-  <dimension ref="A1:N22"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC6C22-F4D3-4FD5-B3E7-30320A6E2BB0}">
+  <dimension ref="A2:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="5" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="130" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="130" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="131" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="131" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="131" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="131" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="131" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="131" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-    </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="120"/>
-      <c r="B2" s="129" t="s">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="132">
-        <v>2.5</v>
-      </c>
-      <c r="D2" s="132">
+      <c r="F2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="132">
-        <v>48</v>
-      </c>
-      <c r="F2" s="132">
+      <c r="G2" s="103" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="104" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="106" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="108" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="109" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="140" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="126">
+        <v>0.86423333300000005</v>
+      </c>
+      <c r="B3" s="126">
+        <v>108.9092</v>
+      </c>
+      <c r="C3" s="127">
+        <f>SUM(E3:N8)</f>
+        <v>956.90000000000009</v>
+      </c>
+      <c r="D3" s="119" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="110"/>
+      <c r="F3" s="111">
+        <f>100+100</f>
+        <v>200</v>
+      </c>
+      <c r="G3" s="112"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="115">
+        <v>90</v>
+      </c>
+      <c r="K3" s="116"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="141"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="126">
+        <v>4.5260000000000002E-2</v>
+      </c>
+      <c r="B4" s="126">
+        <v>109.23968000000001</v>
+      </c>
+      <c r="D4" s="119" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="110">
+        <v>15</v>
+      </c>
+      <c r="F4" s="111"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="141"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="126">
+        <v>1.1174249999999999</v>
+      </c>
+      <c r="B5" s="126">
+        <v>109.55835</v>
+      </c>
+      <c r="D5" s="119" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="110"/>
+      <c r="F5" s="111">
+        <v>100</v>
+      </c>
+      <c r="G5" s="112"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="114">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="115"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="141">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="126">
+        <v>0.17745</v>
+      </c>
+      <c r="B6" s="126">
+        <v>110.0471</v>
+      </c>
+      <c r="D6" s="119" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="110">
+        <v>7</v>
+      </c>
+      <c r="F6" s="111"/>
+      <c r="G6" s="112">
+        <v>100</v>
+      </c>
+      <c r="H6" s="113"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="118"/>
+      <c r="N6" s="141"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="126">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="B7" s="126">
+        <v>110.9554667</v>
+      </c>
+      <c r="D7" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="110"/>
+      <c r="F7" s="111">
+        <f>14+21</f>
+        <v>35</v>
+      </c>
+      <c r="G7" s="112"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="114">
+        <f>1.2+0.4</f>
+        <v>1.6</v>
+      </c>
+      <c r="J7" s="115">
+        <f>6+7.7+12.9+13+4+6.2+4+3.5+12+8+9+8+2</f>
+        <v>96.300000000000011</v>
+      </c>
+      <c r="K7" s="116"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="141"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="126">
+        <v>-1.7742</v>
+      </c>
+      <c r="B8" s="126">
+        <v>110.0303</v>
+      </c>
+      <c r="D8" s="119" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="110">
+        <v>7</v>
+      </c>
+      <c r="F8" s="111">
+        <f>20</f>
         <v>20</v>
       </c>
-      <c r="G2" s="120">
-        <f>0.5*1000</f>
-        <v>500</v>
-      </c>
-      <c r="H2" s="132">
-        <v>0.04</v>
-      </c>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="120"/>
-      <c r="B3" s="129" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="132">
-        <v>1.65</v>
-      </c>
-      <c r="D3" s="132">
-        <v>0.13</v>
-      </c>
-      <c r="E3" s="132">
-        <v>45</v>
-      </c>
-      <c r="F3" s="132">
+      <c r="G8" s="112"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="115">
+        <f>23+1.2+2.8+0.8+5.9+10+3.5+6+1</f>
+        <v>54.2</v>
+      </c>
+      <c r="K8" s="116"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="141"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="126">
+        <v>-2.6152000000000002</v>
+      </c>
+      <c r="B9" s="126">
+        <v>111.7037</v>
+      </c>
+      <c r="C9" s="127">
+        <f>SUM(E9:N13)</f>
+        <v>734</v>
+      </c>
+      <c r="D9" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="110"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="115">
+        <f>6+10+3</f>
+        <v>19</v>
+      </c>
+      <c r="K9" s="116"/>
+      <c r="L9" s="117"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="141"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="126">
+        <v>-2.6220500000000002</v>
+      </c>
+      <c r="B10" s="126">
+        <v>112.91540000000001</v>
+      </c>
+      <c r="D10" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="110"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="115">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="K10" s="116"/>
+      <c r="L10" s="117"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="141"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="126">
+        <v>-2.1166</v>
+      </c>
+      <c r="B11" s="126">
+        <v>113.7459333</v>
+      </c>
+      <c r="D11" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="110"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="115">
+        <f>5+34+2</f>
+        <v>41</v>
+      </c>
+      <c r="K11" s="116"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="141"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="126">
+        <v>-2.8550333330000002</v>
+      </c>
+      <c r="B12" s="126">
+        <v>114.2789667</v>
+      </c>
+      <c r="D12" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="110"/>
+      <c r="F12" s="111">
+        <v>120</v>
+      </c>
+      <c r="G12" s="112"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="118"/>
+      <c r="N12" s="141"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="126">
+        <v>-0.74419999999999997</v>
+      </c>
+      <c r="B13" s="126">
+        <v>115.00215</v>
+      </c>
+      <c r="D13" s="119" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="110">
+        <f>9</f>
+        <v>9</v>
+      </c>
+      <c r="F13" s="111">
+        <f>211</f>
+        <v>211</v>
+      </c>
+      <c r="G13" s="112">
+        <f>156+140</f>
+        <v>296</v>
+      </c>
+      <c r="H13" s="113"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="115">
+        <f>21+4+5</f>
+        <v>30</v>
+      </c>
+      <c r="K13" s="116"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="118"/>
+      <c r="N13" s="141"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="126">
+        <v>-3.4291333329999998</v>
+      </c>
+      <c r="B14" s="126">
+        <v>114.7738222</v>
+      </c>
+      <c r="C14" s="127">
+        <f>SUM(E14:N16)</f>
+        <v>666.94</v>
+      </c>
+      <c r="D14" s="119" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="110"/>
+      <c r="F14" s="111">
+        <f>55</f>
+        <v>55</v>
+      </c>
+      <c r="G14" s="112">
+        <v>21</v>
+      </c>
+      <c r="H14" s="113"/>
+      <c r="I14" s="114">
+        <v>30</v>
+      </c>
+      <c r="J14" s="115">
+        <v>87.74</v>
+      </c>
+      <c r="K14" s="116"/>
+      <c r="L14" s="117"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="141"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="126">
+        <v>-2.26065</v>
+      </c>
+      <c r="B15" s="126">
+        <v>115.26295</v>
+      </c>
+      <c r="D15" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="110"/>
+      <c r="F15" s="111">
+        <v>260</v>
+      </c>
+      <c r="G15" s="112"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="115">
+        <f>6.81+2.12</f>
+        <v>8.93</v>
+      </c>
+      <c r="K15" s="116"/>
+      <c r="L15" s="117"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="141"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="126">
+        <v>-3.5974499999999998</v>
+      </c>
+      <c r="B16" s="126">
+        <v>115.7526</v>
+      </c>
+      <c r="D16" s="119" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="110"/>
+      <c r="F16" s="111">
+        <v>200</v>
+      </c>
+      <c r="G16" s="112"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="115">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="K16" s="116"/>
+      <c r="L16" s="117"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="141"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="126">
+        <v>-1.761425</v>
+      </c>
+      <c r="B17" s="126">
+        <v>116.11315</v>
+      </c>
+      <c r="C17" s="127">
+        <f>SUM(E17:M21)</f>
+        <v>1523.4</v>
+      </c>
+      <c r="D17" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="110"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="114"/>
+      <c r="J17" s="115">
+        <f>133.3+20+44.5</f>
+        <v>197.8</v>
+      </c>
+      <c r="K17" s="116"/>
+      <c r="L17" s="117"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="141"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="126">
+        <v>-1.190416667</v>
+      </c>
+      <c r="B18" s="126">
+        <v>116.87775000000001</v>
+      </c>
+      <c r="D18" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="110"/>
+      <c r="F18" s="111">
+        <f>220+50</f>
+        <v>270</v>
+      </c>
+      <c r="G18" s="112">
+        <f>200+80+53.1+82+35+4</f>
+        <v>454.1</v>
+      </c>
+      <c r="H18" s="113"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="115"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="117"/>
+      <c r="M18" s="118"/>
+      <c r="N18" s="141"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="126">
+        <v>-0.48473333299999999</v>
+      </c>
+      <c r="B19" s="126">
+        <v>117.0814444</v>
+      </c>
+      <c r="D19" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="110"/>
+      <c r="F19" s="111">
+        <v>550</v>
+      </c>
+      <c r="G19" s="112"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="115"/>
+      <c r="K19" s="116"/>
+      <c r="L19" s="117"/>
+      <c r="M19" s="118"/>
+      <c r="N19" s="141"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="126">
+        <v>0.31574999999999998</v>
+      </c>
+      <c r="B20" s="126">
+        <v>117.50215</v>
+      </c>
+      <c r="D20" s="119" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="110"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="114"/>
+      <c r="J20" s="115">
+        <f>4.4+3.8+7.8</f>
+        <v>16</v>
+      </c>
+      <c r="K20" s="116"/>
+      <c r="L20" s="117"/>
+      <c r="M20" s="118"/>
+      <c r="N20" s="141"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="126">
+        <v>1.0532999999999999</v>
+      </c>
+      <c r="B21" s="126">
+        <v>116.92149999999999</v>
+      </c>
+      <c r="D21" s="119" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="110"/>
+      <c r="F21" s="111">
+        <f>15</f>
+        <v>15</v>
+      </c>
+      <c r="G21" s="112"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="114"/>
+      <c r="J21" s="115">
+        <f>16.1+4.4</f>
+        <v>20.5</v>
+      </c>
+      <c r="K21" s="116"/>
+      <c r="L21" s="117"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="141"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="126">
+        <v>3.2987666670000002</v>
+      </c>
+      <c r="B22" s="126">
+        <v>116.9458333</v>
+      </c>
+      <c r="C22" s="127">
+        <f>SUM(E22:N22)</f>
+        <v>175.55</v>
+      </c>
+      <c r="D22" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="120">
-        <v>849</v>
-      </c>
-      <c r="H3" s="132">
-        <v>0.01</v>
-      </c>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="129" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="132">
-        <v>0.75</v>
-      </c>
-      <c r="D4" s="132">
-        <v>2.5</v>
-      </c>
-      <c r="E4" s="132">
-        <v>23</v>
-      </c>
-      <c r="F4" s="132">
-        <v>30</v>
-      </c>
-      <c r="G4" s="120">
-        <v>433</v>
-      </c>
-      <c r="H4" s="132">
-        <v>0.12</v>
-      </c>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="120"/>
-      <c r="B5" s="129" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="132">
-        <v>4.5</v>
-      </c>
-      <c r="D5" s="132">
-        <v>0.37</v>
-      </c>
-      <c r="E5" s="132">
-        <v>20</v>
-      </c>
-      <c r="F5" s="132">
-        <v>30</v>
-      </c>
-      <c r="G5" s="120">
+      <c r="E22" s="110"/>
+      <c r="F22" s="111">
+        <f>5+3.5+17</f>
+        <v>25.5</v>
+      </c>
+      <c r="G22" s="112">
+        <f>17.82+12+5+6+24.4+10</f>
+        <v>75.22</v>
+      </c>
+      <c r="H22" s="113"/>
+      <c r="I22" s="114"/>
+      <c r="J22" s="115">
+        <f>13.26+17.43+12+4.96+7.63+16.4+2.35+0.8</f>
+        <v>74.83</v>
+      </c>
+      <c r="K22" s="116"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="141"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D23" s="125">
+        <f>SUM(E23:M23)</f>
+        <v>3826.7900000000004</v>
+      </c>
+      <c r="E23" s="123">
+        <f>SUM(E3:E22)</f>
         <v>38</v>
       </c>
-      <c r="H5" s="132">
-        <v>0.2</v>
-      </c>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="129" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="132">
-        <v>1.9</v>
-      </c>
-      <c r="D6" s="132">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="132">
-        <v>53</v>
-      </c>
-      <c r="F6" s="132">
-        <v>80</v>
-      </c>
-      <c r="G6" s="120">
-        <v>6</v>
-      </c>
-      <c r="H6" s="132">
-        <v>0.3</v>
-      </c>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-      <c r="N6" s="120"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="120"/>
-      <c r="B7" s="129" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="132">
-        <v>1</v>
-      </c>
-      <c r="D7" s="132">
-        <v>2.4</v>
-      </c>
-      <c r="E7" s="132">
-        <f>0.02*1000</f>
-        <v>20</v>
-      </c>
-      <c r="F7" s="132">
-        <v>25</v>
-      </c>
-      <c r="G7" s="120">
-        <v>600</v>
-      </c>
-      <c r="H7" s="132">
-        <v>0.04</v>
-      </c>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="120"/>
-      <c r="N7" s="120"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="129" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="132">
-        <v>0.7</v>
-      </c>
-      <c r="D8" s="132">
-        <v>0</v>
-      </c>
-      <c r="E8" s="132">
-        <v>15</v>
-      </c>
-      <c r="F8" s="132">
-        <v>25</v>
-      </c>
-      <c r="G8" s="120">
-        <v>7</v>
-      </c>
-      <c r="H8" s="120"/>
-      <c r="I8" s="120"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="120"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="129" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-      <c r="N9" s="120"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="129" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="132">
-        <v>1.88</v>
-      </c>
-      <c r="D10" s="132">
-        <v>0</v>
-      </c>
-      <c r="E10" s="132">
-        <v>60</v>
-      </c>
-      <c r="F10" s="132">
-        <v>25</v>
-      </c>
-      <c r="G10" s="120">
-        <v>8</v>
-      </c>
-      <c r="H10" s="120"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
-      <c r="B11" s="133" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="132">
-        <v>4</v>
-      </c>
-      <c r="D11" s="132">
-        <v>0</v>
-      </c>
-      <c r="E11" s="132">
-        <v>124</v>
-      </c>
-      <c r="F11" s="132">
-        <v>25</v>
-      </c>
-      <c r="G11" s="120">
-        <v>12</v>
-      </c>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="120"/>
-      <c r="M11" s="120"/>
-      <c r="N11" s="120"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
-      <c r="B12" s="120"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="120"/>
-      <c r="E12" s="120"/>
-      <c r="F12" s="120"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="120"/>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="120"/>
-      <c r="N12" s="120"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="130" t="s">
+      <c r="F23" s="123">
+        <f t="shared" ref="F23:M23" si="0">SUM(F3:F22)</f>
+        <v>2061.5</v>
+      </c>
+      <c r="G23" s="123">
+        <f t="shared" si="0"/>
+        <v>946.32</v>
+      </c>
+      <c r="H23" s="123">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="123">
+        <f t="shared" si="0"/>
+        <v>32.4</v>
+      </c>
+      <c r="J23" s="123">
+        <f>SUM(J3:J22)</f>
+        <v>748.57</v>
+      </c>
+      <c r="K23" s="123">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="123">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="123">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="127">
+        <f t="shared" ref="N23" si="1">SUM(N3:N22)</f>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="127"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
-      <c r="L13" s="120"/>
-      <c r="M13" s="120"/>
-      <c r="N13" s="120"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="120"/>
-      <c r="N14" s="120"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="120" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
-      <c r="L15" s="120"/>
-      <c r="M15" s="120"/>
-      <c r="N15" s="120"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="120" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-      <c r="N16" s="120"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="120" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120"/>
-      <c r="K17" s="120"/>
-      <c r="L17" s="120"/>
-      <c r="M17" s="120"/>
-      <c r="N17" s="120"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="120" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="120"/>
-      <c r="C18" s="120"/>
-      <c r="D18" s="120"/>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120"/>
-      <c r="G18" s="120"/>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
-      <c r="J18" s="120"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="120"/>
-      <c r="N18" s="120"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="120" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="120"/>
-      <c r="C19" s="120"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="120"/>
-      <c r="K19" s="120"/>
-      <c r="L19" s="120"/>
-      <c r="M19" s="120"/>
-      <c r="N19" s="120"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="120"/>
-      <c r="B20" s="120"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="120"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="120"/>
-      <c r="K20" s="120"/>
-      <c r="L20" s="120"/>
-      <c r="M20" s="120"/>
-      <c r="N20" s="120"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="120"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="120"/>
-      <c r="F21" s="120"/>
-      <c r="G21" s="120"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="120"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="120"/>
-      <c r="N21" s="120"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="120"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="120"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="120"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="120"/>
-      <c r="N22" s="120"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A63535-D95A-4D36-8C1E-9289FDA2D070}">
   <dimension ref="A1:AE93"/>
   <sheetViews>
@@ -8365,39 +9048,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" s="142" t="s">
+      <c r="E1" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142"/>
-      <c r="M1" s="142"/>
-      <c r="N1" s="142" t="s">
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="142"/>
-      <c r="P1" s="142"/>
-      <c r="Q1" s="142"/>
-      <c r="R1" s="142"/>
-      <c r="S1" s="142"/>
-      <c r="T1" s="142"/>
-      <c r="U1" s="142"/>
-      <c r="V1" s="142"/>
-      <c r="W1" s="149" t="s">
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="144"/>
+      <c r="R1" s="144"/>
+      <c r="S1" s="144"/>
+      <c r="T1" s="144"/>
+      <c r="U1" s="144"/>
+      <c r="V1" s="144"/>
+      <c r="W1" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="149"/>
-      <c r="Y1" s="149"/>
-      <c r="Z1" s="149"/>
-      <c r="AA1" s="149"/>
-      <c r="AB1" s="149"/>
-      <c r="AC1" s="149"/>
-      <c r="AD1" s="149"/>
-      <c r="AE1" s="149"/>
+      <c r="X1" s="151"/>
+      <c r="Y1" s="151"/>
+      <c r="Z1" s="151"/>
+      <c r="AA1" s="151"/>
+      <c r="AB1" s="151"/>
+      <c r="AC1" s="151"/>
+      <c r="AD1" s="151"/>
+      <c r="AE1" s="151"/>
     </row>
     <row r="2" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -8498,7 +9181,7 @@
       <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="146">
+      <c r="D3" s="148">
         <v>1</v>
       </c>
       <c r="E3" s="83">
@@ -8590,7 +9273,7 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="147"/>
+      <c r="D4" s="149"/>
       <c r="E4" s="85"/>
       <c r="F4" s="36"/>
       <c r="G4" s="37"/>
@@ -8623,7 +9306,7 @@
       <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="147"/>
+      <c r="D5" s="149"/>
       <c r="E5" s="85"/>
       <c r="F5" s="36"/>
       <c r="G5" s="37"/>
@@ -8656,7 +9339,7 @@
       <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="147"/>
+      <c r="D6" s="149"/>
       <c r="E6" s="85"/>
       <c r="F6" s="36"/>
       <c r="G6" s="37"/>
@@ -8689,7 +9372,7 @@
       <c r="C7" s="3">
         <v>4</v>
       </c>
-      <c r="D7" s="147"/>
+      <c r="D7" s="149"/>
       <c r="E7" s="85"/>
       <c r="F7" s="36"/>
       <c r="G7" s="37"/>
@@ -8722,7 +9405,7 @@
       <c r="C8" s="3">
         <v>5</v>
       </c>
-      <c r="D8" s="147"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="85"/>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
@@ -8755,7 +9438,7 @@
       <c r="C9" s="3">
         <v>11</v>
       </c>
-      <c r="D9" s="148"/>
+      <c r="D9" s="150"/>
       <c r="E9" s="87"/>
       <c r="F9" s="46"/>
       <c r="G9" s="47"/>
@@ -8788,7 +9471,7 @@
       <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="D10" s="146">
+      <c r="D10" s="148">
         <v>2</v>
       </c>
       <c r="E10" s="83">
@@ -8879,7 +9562,7 @@
       <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="148"/>
+      <c r="D11" s="150"/>
       <c r="E11" s="87"/>
       <c r="F11" s="46"/>
       <c r="G11" s="47"/>
@@ -8912,7 +9595,7 @@
       <c r="C12" s="1">
         <v>6</v>
       </c>
-      <c r="D12" s="146">
+      <c r="D12" s="148">
         <v>3</v>
       </c>
       <c r="E12" s="83">
@@ -9003,7 +9686,7 @@
       <c r="C13" s="1">
         <v>7</v>
       </c>
-      <c r="D13" s="147"/>
+      <c r="D13" s="149"/>
       <c r="E13" s="85"/>
       <c r="F13" s="36"/>
       <c r="G13" s="37"/>
@@ -9036,7 +9719,7 @@
       <c r="C14" s="1">
         <v>8</v>
       </c>
-      <c r="D14" s="148"/>
+      <c r="D14" s="150"/>
       <c r="E14" s="87"/>
       <c r="F14" s="46"/>
       <c r="G14" s="47"/>
@@ -9075,7 +9758,7 @@
       <c r="C15" s="6">
         <v>13</v>
       </c>
-      <c r="D15" s="146">
+      <c r="D15" s="148">
         <v>4</v>
       </c>
       <c r="E15" s="83">
@@ -9163,7 +9846,7 @@
       <c r="C16" s="6">
         <v>14</v>
       </c>
-      <c r="D16" s="147"/>
+      <c r="D16" s="149"/>
       <c r="E16" s="85"/>
       <c r="F16" s="36"/>
       <c r="G16" s="37"/>
@@ -9196,7 +9879,7 @@
       <c r="C17" s="6">
         <v>15</v>
       </c>
-      <c r="D17" s="148"/>
+      <c r="D17" s="150"/>
       <c r="E17" s="87"/>
       <c r="F17" s="46"/>
       <c r="G17" s="47"/>
@@ -9235,7 +9918,7 @@
       <c r="C18" s="7">
         <v>16</v>
       </c>
-      <c r="D18" s="146">
+      <c r="D18" s="148">
         <v>5</v>
       </c>
       <c r="E18" s="83"/>
@@ -9320,7 +10003,7 @@
       <c r="C19" s="7">
         <v>17</v>
       </c>
-      <c r="D19" s="147"/>
+      <c r="D19" s="149"/>
       <c r="E19" s="85"/>
       <c r="F19" s="36"/>
       <c r="G19" s="37"/>
@@ -9353,7 +10036,7 @@
       <c r="C20" s="7">
         <v>18</v>
       </c>
-      <c r="D20" s="147"/>
+      <c r="D20" s="149"/>
       <c r="E20" s="85"/>
       <c r="F20" s="36"/>
       <c r="G20" s="37"/>
@@ -9386,7 +10069,7 @@
       <c r="C21" s="7">
         <v>19</v>
       </c>
-      <c r="D21" s="147"/>
+      <c r="D21" s="149"/>
       <c r="E21" s="85"/>
       <c r="F21" s="36"/>
       <c r="G21" s="37"/>
@@ -9419,7 +10102,7 @@
       <c r="C22" s="7">
         <v>20</v>
       </c>
-      <c r="D22" s="147"/>
+      <c r="D22" s="149"/>
       <c r="E22" s="85"/>
       <c r="F22" s="36"/>
       <c r="G22" s="37"/>
@@ -9452,7 +10135,7 @@
       <c r="C23" s="7">
         <v>21</v>
       </c>
-      <c r="D23" s="148"/>
+      <c r="D23" s="150"/>
       <c r="E23" s="87"/>
       <c r="F23" s="46"/>
       <c r="G23" s="47"/>
@@ -9491,7 +10174,7 @@
       <c r="C24" s="8">
         <v>36</v>
       </c>
-      <c r="D24" s="146">
+      <c r="D24" s="148">
         <v>7</v>
       </c>
       <c r="E24" s="83"/>
@@ -9580,7 +10263,7 @@
       <c r="C25" s="8">
         <v>37</v>
       </c>
-      <c r="D25" s="147"/>
+      <c r="D25" s="149"/>
       <c r="E25" s="85"/>
       <c r="F25" s="36"/>
       <c r="G25" s="37"/>
@@ -9613,7 +10296,7 @@
       <c r="C26" s="8">
         <v>38</v>
       </c>
-      <c r="D26" s="148"/>
+      <c r="D26" s="150"/>
       <c r="E26" s="87"/>
       <c r="F26" s="46"/>
       <c r="G26" s="47"/>
@@ -9743,7 +10426,7 @@
       <c r="C28" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="146">
+      <c r="D28" s="148">
         <v>8</v>
       </c>
       <c r="E28" s="83"/>
@@ -9830,7 +10513,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C29" s="17"/>
-      <c r="D29" s="147"/>
+      <c r="D29" s="149"/>
       <c r="E29" s="85"/>
       <c r="F29" s="36"/>
       <c r="G29" s="37"/>
@@ -9861,7 +10544,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C30" s="17"/>
-      <c r="D30" s="147"/>
+      <c r="D30" s="149"/>
       <c r="E30" s="85"/>
       <c r="F30" s="36"/>
       <c r="G30" s="37"/>
@@ -9892,7 +10575,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C31" s="17"/>
-      <c r="D31" s="147"/>
+      <c r="D31" s="149"/>
       <c r="E31" s="85"/>
       <c r="F31" s="36"/>
       <c r="G31" s="37"/>
@@ -9923,7 +10606,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C32" s="17"/>
-      <c r="D32" s="147"/>
+      <c r="D32" s="149"/>
       <c r="E32" s="85"/>
       <c r="F32" s="36"/>
       <c r="G32" s="37"/>
@@ -9954,7 +10637,7 @@
     </row>
     <row r="33" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="17"/>
-      <c r="D33" s="148"/>
+      <c r="D33" s="150"/>
       <c r="E33" s="87"/>
       <c r="F33" s="46"/>
       <c r="G33" s="47"/>
@@ -9993,7 +10676,7 @@
       <c r="C34" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="146">
+      <c r="D34" s="148">
         <v>9</v>
       </c>
       <c r="E34" s="83">
@@ -10082,7 +10765,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C35" s="25"/>
-      <c r="D35" s="147"/>
+      <c r="D35" s="149"/>
       <c r="E35" s="85"/>
       <c r="F35" s="36"/>
       <c r="G35" s="37"/>
@@ -10113,7 +10796,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C36" s="25"/>
-      <c r="D36" s="147"/>
+      <c r="D36" s="149"/>
       <c r="E36" s="85"/>
       <c r="F36" s="36"/>
       <c r="G36" s="37"/>
@@ -10144,7 +10827,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C37" s="25"/>
-      <c r="D37" s="147"/>
+      <c r="D37" s="149"/>
       <c r="E37" s="85"/>
       <c r="F37" s="36"/>
       <c r="G37" s="37"/>
@@ -10175,7 +10858,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C38" s="25"/>
-      <c r="D38" s="147"/>
+      <c r="D38" s="149"/>
       <c r="E38" s="85"/>
       <c r="F38" s="36"/>
       <c r="G38" s="37"/>
@@ -10206,7 +10889,7 @@
     </row>
     <row r="39" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39" s="25"/>
-      <c r="D39" s="148"/>
+      <c r="D39" s="150"/>
       <c r="E39" s="87"/>
       <c r="F39" s="46"/>
       <c r="G39" s="47"/>

</xml_diff>

<commit_message>
sixteenth update: GL preparation
</commit_message>
<xml_diff>
--- a/database/calliope_generators.xlsx
+++ b/database/calliope_generators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_energy_transition\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D370A1-10F8-4F6B-92A5-260562CA1AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED53980-0B1F-460A-910F-C51C48658865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{15FFB4DA-647B-47A8-A954-D576C3956A52}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -3637,7 +3637,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3745,8 +3745,8 @@
         <v>849</v>
       </c>
       <c r="H3" s="34">
-        <f>0.01*60</f>
-        <v>0.6</v>
+        <f>0.04*60</f>
+        <v>2.4</v>
       </c>
       <c r="I3" s="34">
         <v>0.8</v>
@@ -9325,7 +9325,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14200,11 +14200,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:BA61"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="AZ16" sqref="AZ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19098,11 +19098,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3A25C5-56EB-4173-9671-DD148E735217}">
   <dimension ref="A1:BA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>